<commit_message>
AutoCommit_27 сентября 2023 г. 9:06:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Дз3</t>
+  </si>
+  <si>
+    <t>Дз4</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +194,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -208,6 +222,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -515,10 +532,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -553,7 +570,8 @@
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
     </row>
-    <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
@@ -563,8 +581,11 @@
       <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -614,6 +635,9 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -665,7 +689,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -676,7 +700,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -687,9 +711,14 @@
         <v>33</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -713,7 +742,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -724,7 +753,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -737,7 +766,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -750,7 +779,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -761,9 +790,11 @@
         <v>33</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -774,7 +805,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -787,7 +818,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -797,12 +828,17 @@
       <c r="C23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -813,7 +849,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -826,9 +862,11 @@
       <c r="D25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -841,7 +879,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -854,9 +892,14 @@
       <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -867,7 +910,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -878,7 +921,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -889,18 +932,27 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -911,7 +963,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -924,18 +976,25 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C35" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_2 октября 2023 г. 10:06:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -220,11 +220,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -532,10 +532,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -546,29 +546,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -633,8 +633,12 @@
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F8" t="s">
         <v>33</v>
       </c>
@@ -834,7 +838,7 @@
       <c r="E23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -895,7 +899,7 @@
       <c r="E27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_2 октября 2023 г. 10:15:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -535,7 +535,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -757,7 +757,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -780,10 +780,17 @@
       <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 октября 2023 г. 8:21:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -535,7 +535,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -678,7 +678,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -691,7 +691,12 @@
       <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -714,11 +719,19 @@
       <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_17 октября 2023 г. 10:10:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -532,10 +532,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -783,7 +783,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -803,7 +803,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -818,7 +818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -829,7 +829,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -842,7 +842,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -862,7 +862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -890,7 +890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -922,8 +922,14 @@
       <c r="F27" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+      <c r="G27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -934,7 +940,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -945,7 +951,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -956,7 +962,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -976,7 +982,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_24 октября 2023 г. 9:46:11_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -532,10 +532,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_31 октября 2023 г. 11:43:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -535,7 +535,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -584,6 +584,15 @@
       <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
@@ -734,6 +743,9 @@
       <c r="H14" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="I14" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -759,7 +771,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -770,7 +782,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -783,7 +795,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -803,7 +815,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -818,7 +830,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -829,7 +841,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -840,9 +852,23 @@
         <v>33</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -862,7 +888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -873,7 +899,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -890,7 +916,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -903,7 +929,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -929,7 +955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -940,7 +966,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -951,7 +977,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -962,7 +988,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -982,7 +1008,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_7 ноября 2023 г. 17:19:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -532,10 +532,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -899,7 +899,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -913,6 +913,9 @@
         <v>33</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1030,7 +1033,9 @@
         <v>33</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 11:26:39_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -535,7 +535,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -887,6 +887,15 @@
       <c r="F23" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1011,7 +1020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1022,7 +1031,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -1036,8 +1045,11 @@
       <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -1055,7 +1067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C35" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 11:28:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -171,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -205,11 +205,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -221,6 +230,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -535,7 +547,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -546,29 +558,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -904,9 +916,24 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -924,7 +951,16 @@
       <c r="E25" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="F25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 11:32:30_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -544,7 +544,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
@@ -633,7 +633,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -644,7 +644,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -663,8 +663,17 @@
       <c r="F8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="G8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1025,7 +1034,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1036,7 +1045,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1053,6 +1062,15 @@
         <v>33</v>
       </c>
       <c r="F31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1063,9 +1081,24 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 12:16:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,7 +547,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1114,6 +1114,9 @@
       <c r="E33" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H33" s="2" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 18:20:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Балашова Алиса</t>
   </si>
   <si>
-    <t>Н</t>
-  </si>
-  <si>
     <t>Бернакевич Елена</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Рублева Маргарита</t>
   </si>
   <si>
-    <t>Саргас Кирилл</t>
-  </si>
-  <si>
     <t>Соди Гитанджелина</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>Дз1.1</t>
   </si>
   <si>
-    <t>ок</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                                                                                                                                                                                                           </t>
   </si>
   <si>
@@ -133,6 +124,9 @@
   </si>
   <si>
     <t>Дз4</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -218,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -235,8 +229,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -544,10 +542,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -558,43 +556,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -618,9 +616,18 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
+      <c r="K5">
+        <f>SUM(C5:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -629,9 +636,18 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
+      <c r="K6" s="6">
+        <f t="shared" ref="K6:K34" si="0">SUM(C6:I6)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -640,9 +656,18 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
+      <c r="K7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -651,26 +676,33 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>33</v>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -680,52 +712,84 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
+      <c r="C9" s="2">
+        <v>5</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+      <c r="K9" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
+      <c r="K10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
+      <c r="K11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -733,39 +797,53 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
+      <c r="K13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -773,373 +851,514 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
+      <c r="K15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="K16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>19</v>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5</v>
+      </c>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4">
+        <v>5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2">
+        <v>5</v>
+      </c>
+      <c r="I25" s="4">
+        <v>5</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="C26" s="2">
+        <v>5</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="K27" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="K28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
+        <v>5</v>
+      </c>
+      <c r="I31" s="2">
+        <v>5</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2">
+        <v>5</v>
+      </c>
+      <c r="H32" s="2">
+        <v>5</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="2">
+        <v>5</v>
+      </c>
+      <c r="G33" s="2">
+        <v>5</v>
+      </c>
+      <c r="H33" s="2">
+        <v>5</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C34" s="2">
+        <v>5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="2">
+        <v>5</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="M34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C35" s="3">
         <v>1</v>
       </c>
@@ -1151,6 +1370,30 @@
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
+  <conditionalFormatting sqref="K5:K34">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M34">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 10:26:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -230,11 +230,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -545,7 +545,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -556,29 +556,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -637,13 +637,26 @@
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
       <c r="K6" s="6">
         <f t="shared" ref="K6:K34" si="0">SUM(C6:I6)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M6">
         <v>2</v>
@@ -891,12 +904,18 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
       <c r="K17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M17">
         <v>2</v>
@@ -1173,7 +1192,7 @@
       <c r="H27" s="2">
         <v>5</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="7"/>
       <c r="K27" s="6">
         <f t="shared" si="0"/>
         <v>30</v>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 11:17:53_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Дз4</t>
-  </si>
-  <si>
-    <t>???</t>
   </si>
 </sst>
 </file>
@@ -542,10 +539,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1043,11 +1040,11 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
+      <c r="A23" s="1">
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2">
         <v>5</v>
@@ -1192,10 +1189,12 @@
       <c r="H27" s="2">
         <v>5</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="7">
+        <v>5</v>
+      </c>
       <c r="K27" s="6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M27">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_14 ноября 2023 г. 11:48:45_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Дз1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                                                                                                                                           </t>
   </si>
   <si>
     <t>Дз2</t>
@@ -539,10 +536,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -583,13 +580,13 @@
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -735,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -743,13 +740,29 @@
         <v>6</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
       <c r="K10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M10">
         <v>2</v>
@@ -809,12 +822,30 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
       <c r="K13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M13">
         <v>2</v>
@@ -863,14 +894,27 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5</v>
+      </c>
+      <c r="G15" s="7">
+        <v>5</v>
+      </c>
+      <c r="H15" s="7">
+        <v>5</v>
+      </c>
       <c r="K15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M15">
         <v>2</v>
@@ -910,9 +954,21 @@
       <c r="E17" s="2">
         <v>5</v>
       </c>
+      <c r="F17" s="4">
+        <v>5</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5</v>
+      </c>
+      <c r="I17" s="4">
+        <v>5</v>
+      </c>
       <c r="K17" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="M17">
         <v>2</v>
@@ -979,9 +1035,15 @@
       <c r="E20" s="2">
         <v>5</v>
       </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20" s="7">
+        <v>5</v>
+      </c>
       <c r="K20" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M20">
         <v>3</v>
@@ -1218,19 +1280,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5</v>
+      </c>
       <c r="K29" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M29">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_21 ноября 2023 г. 10:17:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -539,7 +539,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29:I29"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1041,9 +1041,12 @@
       <c r="H20" s="7">
         <v>5</v>
       </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
       <c r="K20" s="6">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C20:J20)</f>
+        <v>25</v>
       </c>
       <c r="M20">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_28 ноября 2023 г. 13:14:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Дз7</t>
+  </si>
+  <si>
+    <t>5.</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -257,6 +266,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -564,10 +577,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H33" activeCellId="3" sqref="H29 H31 H32 H33"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1232,13 +1245,19 @@
       <c r="F19" s="8">
         <v>5</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="G19" s="12">
+        <v>5</v>
+      </c>
+      <c r="H19" s="12">
+        <v>5</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7">

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 11:25:30_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>5.</t>
+  </si>
+  <si>
+    <t>Вариант 2</t>
+  </si>
+  <si>
+    <t>Вариант3</t>
+  </si>
+  <si>
+    <t>Вариант 3</t>
+  </si>
+  <si>
+    <t>Вариант 1</t>
+  </si>
+  <si>
+    <t>Вариант 4</t>
+  </si>
+  <si>
+    <t>Статюгин Александр</t>
   </si>
 </sst>
 </file>
@@ -239,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -264,12 +282,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -574,13 +596,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -591,29 +613,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -659,14 +681,9 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="7">
-        <f>SUM(C5:I5)</f>
-        <v>0</v>
-      </c>
+      <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="7">
-        <v>2</v>
-      </c>
+      <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -705,14 +722,11 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7">
-        <f t="shared" ref="K6:K34" si="0">SUM(C6:I6)</f>
-        <v>30</v>
+      <c r="K6" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="L6" s="7"/>
-      <c r="M6" s="7">
-        <v>2</v>
-      </c>
+      <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -739,14 +753,11 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K7" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="L7" s="7"/>
-      <c r="M7" s="7">
-        <v>2</v>
-      </c>
+      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -787,14 +798,11 @@
         <v>5</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K8" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="L8" s="7"/>
-      <c r="M8" s="7">
-        <v>5</v>
-      </c>
+      <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -823,14 +831,9 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7">
-        <v>3</v>
-      </c>
+      <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -871,14 +874,11 @@
         <v>5</v>
       </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K10" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="L10" s="7"/>
-      <c r="M10" s="7">
-        <v>2</v>
-      </c>
+      <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
@@ -905,14 +905,9 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="7">
-        <v>2</v>
-      </c>
+      <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -947,14 +942,11 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="K12" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="L12" s="7"/>
-      <c r="M12" s="7">
-        <v>5</v>
-      </c>
+      <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
@@ -995,14 +987,11 @@
         <v>5</v>
       </c>
       <c r="J13" s="7"/>
-      <c r="K13" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K13" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="L13" s="7"/>
-      <c r="M13" s="7">
-        <v>2</v>
-      </c>
+      <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -1043,14 +1032,11 @@
         <v>5</v>
       </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K14" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="L14" s="7"/>
-      <c r="M14" s="7">
-        <v>5</v>
-      </c>
+      <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -1089,14 +1075,11 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="K15" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="L15" s="7"/>
-      <c r="M15" s="7">
-        <v>2</v>
-      </c>
+      <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -1123,14 +1106,11 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K16" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="L16" s="7"/>
-      <c r="M16" s="7">
-        <v>2</v>
-      </c>
+      <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -1171,14 +1151,9 @@
         <v>5</v>
       </c>
       <c r="J17" s="7"/>
-      <c r="K17" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
+      <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="7">
-        <v>2</v>
-      </c>
+      <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1207,14 +1182,9 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="7">
-        <v>3</v>
-      </c>
+      <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
@@ -1245,24 +1215,21 @@
       <c r="F19" s="8">
         <v>5</v>
       </c>
-      <c r="G19" s="12">
-        <v>5</v>
-      </c>
-      <c r="H19" s="12">
-        <v>5</v>
-      </c>
-      <c r="I19" s="13" t="s">
+      <c r="G19" s="10">
+        <v>5</v>
+      </c>
+      <c r="H19" s="10">
+        <v>5</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>38</v>
       </c>
       <c r="J19" s="7"/>
-      <c r="K19" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="K19" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="L19" s="7"/>
-      <c r="M19" s="7">
-        <v>5</v>
-      </c>
+      <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
@@ -1299,14 +1266,11 @@
       <c r="J20" s="7">
         <v>5</v>
       </c>
-      <c r="K20" s="7">
-        <f>SUM(C20:J20)</f>
-        <v>25</v>
+      <c r="K20" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="L20" s="7"/>
-      <c r="M20" s="7">
-        <v>3</v>
-      </c>
+      <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -1333,14 +1297,11 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K21" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="L21" s="7"/>
-      <c r="M21" s="7">
-        <v>2</v>
-      </c>
+      <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -1379,14 +1340,11 @@
         <v>5</v>
       </c>
       <c r="J22" s="7"/>
-      <c r="K22" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="K22" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="L22" s="7"/>
-      <c r="M22" s="7">
-        <v>5</v>
-      </c>
+      <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -1427,14 +1385,11 @@
         <v>5</v>
       </c>
       <c r="J23" s="7"/>
-      <c r="K23" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K23" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="L23" s="7"/>
-      <c r="M23" s="7">
-        <v>5</v>
-      </c>
+      <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -1473,14 +1428,9 @@
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
+      <c r="K24" s="7"/>
       <c r="L24" s="7"/>
-      <c r="M24" s="7">
-        <v>5</v>
-      </c>
+      <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -1521,14 +1471,11 @@
         <v>5</v>
       </c>
       <c r="J25" s="7"/>
-      <c r="K25" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K25" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="7">
-        <v>5</v>
-      </c>
+      <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -1567,14 +1514,9 @@
         <v>5</v>
       </c>
       <c r="J26" s="7"/>
-      <c r="K26" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
+      <c r="K26" s="7"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="7">
-        <v>3</v>
-      </c>
+      <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -1615,14 +1557,11 @@
         <v>5</v>
       </c>
       <c r="J27" s="7"/>
-      <c r="K27" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K27" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="L27" s="7"/>
-      <c r="M27" s="7">
-        <v>5</v>
-      </c>
+      <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
@@ -1649,14 +1588,9 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="7">
-        <v>2</v>
-      </c>
+      <c r="M28" s="7"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
@@ -1697,14 +1631,9 @@
         <v>5</v>
       </c>
       <c r="J29" s="7"/>
-      <c r="K29" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
+      <c r="K29" s="7"/>
       <c r="L29" s="7"/>
-      <c r="M29" s="7">
-        <v>2</v>
-      </c>
+      <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
@@ -1731,14 +1660,11 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="K30" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="L30" s="7"/>
-      <c r="M30" s="7">
-        <v>2</v>
-      </c>
+      <c r="M30" s="7"/>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
@@ -1779,14 +1705,11 @@
         <v>5</v>
       </c>
       <c r="J31" s="7"/>
-      <c r="K31" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="K31" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="L31" s="7"/>
-      <c r="M31" s="7">
-        <v>5</v>
-      </c>
+      <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
@@ -1825,14 +1748,11 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
-      <c r="K32" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="K32" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="L32" s="7"/>
-      <c r="M32" s="7">
-        <v>5</v>
-      </c>
+      <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
@@ -1867,14 +1787,11 @@
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-      <c r="K33" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="K33" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="L33" s="7"/>
-      <c r="M33" s="7">
-        <v>5</v>
-      </c>
+      <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
@@ -1907,14 +1824,9 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
-      <c r="K34" s="7">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
+      <c r="K34" s="7"/>
       <c r="L34" s="7"/>
-      <c r="M34" s="7">
-        <v>5</v>
-      </c>
+      <c r="M34" s="7"/>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
@@ -1933,12 +1845,32 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
+    <row r="36" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:K34">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5:M34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1950,7 +1882,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M34">
+  <conditionalFormatting sqref="K36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_5 декабря 2023 г. 18:24:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -602,7 +602,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -831,7 +831,9 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -1251,11 +1253,15 @@
       <c r="C20" s="8">
         <v>5</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6">
+        <v>5</v>
+      </c>
       <c r="E20" s="8">
         <v>5</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="12">
+        <v>5</v>
+      </c>
       <c r="G20" s="8">
         <v>5</v>
       </c>
@@ -1269,7 +1275,9 @@
       <c r="K20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L20" s="7"/>
+      <c r="L20" s="11">
+        <v>5</v>
+      </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -1384,11 +1392,15 @@
       <c r="I23" s="6">
         <v>5</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7" t="s">
+      <c r="J23" s="10">
+        <v>5</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="7"/>
+      <c r="L23" s="10">
+        <v>5</v>
+      </c>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -1704,11 +1716,15 @@
       <c r="I31" s="6">
         <v>5</v>
       </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7" t="s">
+      <c r="J31" s="10">
+        <v>8</v>
+      </c>
+      <c r="K31" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L31" s="7"/>
+      <c r="L31" s="10">
+        <v>9</v>
+      </c>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_6 декабря 2023 г. 11:25:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -138,22 +138,16 @@
     <t>5.</t>
   </si>
   <si>
-    <t>Вариант 2</t>
-  </si>
-  <si>
-    <t>Вариант3</t>
-  </si>
-  <si>
-    <t>Вариант 3</t>
-  </si>
-  <si>
-    <t>Вариант 1</t>
-  </si>
-  <si>
-    <t>Вариант 4</t>
-  </si>
-  <si>
     <t>Статюгин Александр</t>
+  </si>
+  <si>
+    <t>Дз8</t>
+  </si>
+  <si>
+    <t>Дз9</t>
+  </si>
+  <si>
+    <t>Вариант</t>
   </si>
 </sst>
 </file>
@@ -204,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -253,11 +247,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -288,6 +293,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -598,11 +608,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -613,29 +623,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -660,11 +670,48 @@
       <c r="I3" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
+      <c r="M4">
+        <f>SUM(M5:M36)</f>
+        <v>6</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" ref="N4:P4" si="0">SUM(N5:N36)</f>
+        <v>5</v>
+      </c>
+      <c r="O4" s="15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P4" s="15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -683,10 +730,22 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="M5">
+        <f>IF($L5=M$3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="14">
+        <f t="shared" ref="N5:P20" si="1">IF($L5=N$3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
@@ -722,14 +781,26 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
+        <v>2</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" ref="M6:P36" si="2">IF($L6=M$3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -753,14 +824,26 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
@@ -798,14 +881,26 @@
         <v>5</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7">
+        <v>4</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -831,14 +926,26 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -876,14 +983,26 @@
         <v>5</v>
       </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -909,10 +1028,22 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="M11" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
@@ -944,14 +1075,26 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7">
+        <v>2</v>
+      </c>
+      <c r="M12" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
@@ -989,14 +1132,26 @@
         <v>5</v>
       </c>
       <c r="J13" s="7"/>
-      <c r="K13" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="12">
+        <v>4</v>
+      </c>
+      <c r="M13" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
@@ -1034,14 +1189,26 @@
         <v>5</v>
       </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7">
+        <v>3</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P14" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
@@ -1077,14 +1244,26 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="12">
+        <v>3</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
@@ -1108,14 +1287,26 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7">
+        <v>4</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
@@ -1155,10 +1346,22 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="M17" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
@@ -1186,10 +1389,22 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="M18" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
@@ -1227,14 +1442,26 @@
         <v>38</v>
       </c>
       <c r="J19" s="7"/>
-      <c r="K19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7">
+        <v>1</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
@@ -1272,16 +1499,28 @@
       <c r="J20" s="7">
         <v>5</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="11">
-        <v>5</v>
-      </c>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="K20" s="11">
+        <v>5</v>
+      </c>
+      <c r="L20" s="7">
+        <v>4</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
@@ -1305,14 +1544,26 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7">
+        <v>3</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
@@ -1348,14 +1599,26 @@
         <v>5</v>
       </c>
       <c r="J22" s="7"/>
-      <c r="K22" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7">
+        <v>3</v>
+      </c>
+      <c r="M22" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P22" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
@@ -1395,16 +1658,28 @@
       <c r="J23" s="10">
         <v>5</v>
       </c>
-      <c r="K23" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L23" s="10">
-        <v>5</v>
-      </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
+      <c r="K23" s="10">
+        <v>5</v>
+      </c>
+      <c r="L23" s="11">
+        <v>3</v>
+      </c>
+      <c r="M23" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P23" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
@@ -1441,11 +1716,25 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
+      <c r="L24" s="12">
+        <v>1</v>
+      </c>
+      <c r="M24" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
@@ -1483,14 +1772,26 @@
         <v>5</v>
       </c>
       <c r="J25" s="7"/>
-      <c r="K25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7">
+        <v>1</v>
+      </c>
+      <c r="M25" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N25" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
@@ -1528,10 +1829,22 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
+      <c r="M26" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
@@ -1569,14 +1882,26 @@
         <v>5</v>
       </c>
       <c r="J27" s="7"/>
-      <c r="K27" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="12">
+        <v>4</v>
+      </c>
+      <c r="M27" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
@@ -1602,10 +1927,22 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
+      <c r="M28" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
@@ -1645,10 +1982,22 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
+      <c r="M29" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
@@ -1672,14 +2021,26 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7">
+        <v>2</v>
+      </c>
+      <c r="M30" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O30" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
@@ -1719,16 +2080,28 @@
       <c r="J31" s="10">
         <v>8</v>
       </c>
-      <c r="K31" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L31" s="10">
+      <c r="K31" s="10">
         <v>9</v>
       </c>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
+      <c r="L31" s="11">
+        <v>3</v>
+      </c>
+      <c r="M31" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P31" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
       <c r="S31" s="7"/>
@@ -1764,14 +2137,26 @@
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
-      <c r="K32" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7">
+        <v>3</v>
+      </c>
+      <c r="M32" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P32" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
@@ -1803,14 +2188,26 @@
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-      <c r="K33" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7">
+        <v>2</v>
+      </c>
+      <c r="M33" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O33" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
@@ -1842,10 +2239,22 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
+      <c r="M34" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
       <c r="S34" s="7"/>
@@ -1860,13 +2269,45 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
+      <c r="M35" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:23" ht="13" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" s="7" t="s">
         <v>39</v>
+      </c>
+      <c r="L36" s="7">
+        <v>2</v>
+      </c>
+      <c r="M36" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O36" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1874,42 +2315,6 @@
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K34">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M34">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 9:38:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -710,7 +710,7 @@
       </c>
       <c r="P4" s="15">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1345,7 +1345,9 @@
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="L17" s="12">
+        <v>4</v>
+      </c>
       <c r="M17" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1360,7 +1362,7 @@
       </c>
       <c r="P17" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
@@ -1828,7 +1830,9 @@
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
+      <c r="L26" s="12">
+        <v>4</v>
+      </c>
       <c r="M26" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1843,7 +1847,7 @@
       </c>
       <c r="P26" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 10:16:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -612,7 +612,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="I27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1882,11 +1882,15 @@
       <c r="H27" s="8">
         <v>5</v>
       </c>
-      <c r="I27" s="3">
-        <v>5</v>
-      </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="I27" s="10">
+        <v>5</v>
+      </c>
+      <c r="J27" s="10">
+        <v>5</v>
+      </c>
+      <c r="K27" s="10">
+        <v>5</v>
+      </c>
       <c r="L27" s="12">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 10:48:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -608,11 +608,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K27" sqref="I27:K27"/>
+      <selection pane="bottomRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,9 @@
       <c r="F12" s="8">
         <v>5</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="10">
+        <v>5</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1096,7 +1098,9 @@
         <v>0</v>
       </c>
       <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="R12" s="7">
+        <v>5</v>
+      </c>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
@@ -1773,8 +1777,12 @@
       <c r="I25" s="3">
         <v>5</v>
       </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
+      <c r="J25" s="10">
+        <v>5</v>
+      </c>
+      <c r="K25" s="10">
+        <v>5</v>
+      </c>
       <c r="L25" s="7">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 11:15:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R12" sqref="R12"/>
+      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1687,9 @@
         <v>0</v>
       </c>
       <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
+      <c r="R23" s="7">
+        <v>5</v>
+      </c>
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 12:28:59_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -612,7 +612,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
+      <selection pane="bottomRight" activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2121,9 @@
         <v>0</v>
       </c>
       <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
+      <c r="R31" s="7">
+        <v>5</v>
+      </c>
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 13:53:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R23" sqref="R23"/>
+      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="N4" s="15">
         <f t="shared" ref="N4:P4" si="0">SUM(N5:N36)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O4" s="15">
         <f t="shared" si="0"/>
@@ -2258,14 +2258,16 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
+      <c r="L34" s="12">
+        <v>2</v>
+      </c>
       <c r="M34" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N34" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34" s="14">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 10:27:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -880,8 +880,12 @@
       <c r="I8" s="6">
         <v>5</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="10">
+        <v>5</v>
+      </c>
+      <c r="K8" s="10">
+        <v>5</v>
+      </c>
       <c r="L8" s="7">
         <v>4</v>
       </c>
@@ -902,7 +906,9 @@
         <v>1</v>
       </c>
       <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="R8" s="7">
+        <v>5</v>
+      </c>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
@@ -1921,7 +1927,9 @@
         <v>1</v>
       </c>
       <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
+      <c r="R27" s="7">
+        <v>5</v>
+      </c>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 11:39:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -612,7 +612,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -698,7 +698,7 @@
       <c r="E4" s="5"/>
       <c r="M4">
         <f>SUM(M5:M36)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N4" s="15">
         <f t="shared" ref="N4:P4" si="0">SUM(N5:N36)</f>
@@ -925,14 +925,30 @@
       <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7">
+        <v>5</v>
+      </c>
+      <c r="I9" s="12">
+        <v>5</v>
+      </c>
+      <c r="J9" s="12">
+        <v>5</v>
+      </c>
+      <c r="K9" s="12">
+        <v>4</v>
+      </c>
       <c r="L9" s="7">
         <v>1</v>
       </c>
@@ -988,8 +1004,12 @@
       <c r="I10" s="6">
         <v>5</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="J10" s="10">
+        <v>5</v>
+      </c>
+      <c r="K10" s="10">
+        <v>5</v>
+      </c>
       <c r="L10" s="7">
         <v>1</v>
       </c>
@@ -1080,10 +1100,18 @@
       <c r="G12" s="10">
         <v>5</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="H12" s="10">
+        <v>5</v>
+      </c>
+      <c r="I12" s="10">
+        <v>5</v>
+      </c>
+      <c r="J12" s="10">
+        <v>5</v>
+      </c>
+      <c r="K12" s="10">
+        <v>5</v>
+      </c>
       <c r="L12" s="7">
         <v>2</v>
       </c>
@@ -1141,8 +1169,12 @@
       <c r="I13" s="6">
         <v>5</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="J13" s="10">
+        <v>5</v>
+      </c>
+      <c r="K13" s="10">
+        <v>5</v>
+      </c>
       <c r="L13" s="12">
         <v>4</v>
       </c>
@@ -1163,7 +1195,9 @@
         <v>1</v>
       </c>
       <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
+      <c r="R13" s="7">
+        <v>5</v>
+      </c>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
@@ -1198,8 +1232,12 @@
       <c r="I14" s="6">
         <v>5</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="J14" s="10">
+        <v>5</v>
+      </c>
+      <c r="K14" s="10">
+        <v>5</v>
+      </c>
       <c r="L14" s="7">
         <v>3</v>
       </c>
@@ -1220,7 +1258,9 @@
         <v>0</v>
       </c>
       <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
+      <c r="R14" s="7">
+        <v>5</v>
+      </c>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
@@ -1252,9 +1292,15 @@
       <c r="H15" s="8">
         <v>5</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="I15" s="3">
+        <v>5</v>
+      </c>
+      <c r="J15" s="10">
+        <v>5</v>
+      </c>
+      <c r="K15" s="10">
+        <v>5</v>
+      </c>
       <c r="L15" s="12">
         <v>3</v>
       </c>
@@ -1507,7 +1553,9 @@
       <c r="H20" s="8">
         <v>5</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="10">
+        <v>5</v>
+      </c>
       <c r="J20" s="7">
         <v>5</v>
       </c>
@@ -1811,7 +1859,9 @@
         <v>0</v>
       </c>
       <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
+      <c r="R25" s="7">
+        <v>5</v>
+      </c>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
@@ -1837,16 +1887,22 @@
       <c r="F26" s="8">
         <v>5</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3">
+        <v>5</v>
+      </c>
       <c r="H26" s="8">
         <v>5</v>
       </c>
       <c r="I26" s="3">
         <v>5</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="12">
+      <c r="J26" s="10">
+        <v>5</v>
+      </c>
+      <c r="K26" s="10">
+        <v>5</v>
+      </c>
+      <c r="L26" s="11">
         <v>4</v>
       </c>
       <c r="M26" s="14">
@@ -1866,7 +1922,9 @@
         <v>1</v>
       </c>
       <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
+      <c r="R26" s="7">
+        <v>5</v>
+      </c>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
@@ -2007,10 +2065,12 @@
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="L29" s="12">
+        <v>1</v>
+      </c>
       <c r="M29" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="14">
         <f t="shared" si="2"/>
@@ -2039,15 +2099,33 @@
       <c r="B30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
+      <c r="C30" s="10">
+        <v>5</v>
+      </c>
+      <c r="D30" s="10">
+        <v>5</v>
+      </c>
+      <c r="E30" s="10">
+        <v>5</v>
+      </c>
+      <c r="F30" s="10">
+        <v>5</v>
+      </c>
+      <c r="G30" s="10">
+        <v>5</v>
+      </c>
+      <c r="H30" s="10">
+        <v>5</v>
+      </c>
+      <c r="I30" s="10">
+        <v>5</v>
+      </c>
+      <c r="J30" s="10">
+        <v>5</v>
+      </c>
+      <c r="K30" s="10">
+        <v>5</v>
+      </c>
       <c r="L30" s="7">
         <v>2</v>
       </c>
@@ -2068,7 +2146,9 @@
         <v>0</v>
       </c>
       <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
+      <c r="R30" s="7">
+        <v>4</v>
+      </c>
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
       <c r="U30" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 16:15:17_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Сташкова Софья</t>
-  </si>
-  <si>
-    <t>Стятюгин Александр</t>
   </si>
   <si>
     <t>Султанов Денис</t>
@@ -262,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -300,6 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -608,11 +606,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -623,61 +621,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>42</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -702,7 +700,7 @@
       </c>
       <c r="N4" s="15">
         <f t="shared" ref="N4:P4" si="0">SUM(N5:N36)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O4" s="15">
         <f t="shared" si="0"/>
@@ -786,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="M6" s="14">
-        <f t="shared" ref="M6:P36" si="2">IF($L6=M$3,1,0)</f>
+        <f t="shared" ref="M6:P34" si="2">IF($L6=M$3,1,0)</f>
         <v>0</v>
       </c>
       <c r="N6" s="14">
@@ -1446,14 +1444,16 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="L18" s="12">
+        <v>2</v>
+      </c>
       <c r="M18" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N18" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="14">
         <f t="shared" si="1"/>
@@ -1497,7 +1497,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -1692,7 +1692,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="8">
         <v>5</v>
@@ -1998,32 +1998,25 @@
       <c r="A28" s="1">
         <v>24</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="14">
+      <c r="B28" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2</v>
+      </c>
+      <c r="M28" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O28" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2040,7 +2033,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="8">
         <v>5</v>
@@ -2097,7 +2090,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="10">
         <v>5</v>
@@ -2160,7 +2153,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="8">
         <v>5</v>
@@ -2223,7 +2216,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="8">
         <v>5</v>
@@ -2278,7 +2271,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="8">
         <v>5</v>
@@ -2329,7 +2322,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="8">
         <v>5</v>
@@ -2379,46 +2372,16 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="M35" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" ht="13" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="L36" s="7">
-        <v>2</v>
-      </c>
-      <c r="M36" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O36" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 22:45:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -607,10 +607,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -923,19 +923,19 @@
       <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
-      <c r="E9" s="6">
-        <v>5</v>
-      </c>
-      <c r="F9" s="7">
-        <v>5</v>
-      </c>
-      <c r="G9" s="7">
-        <v>5</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="D9" s="8">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="9">
         <v>5</v>
       </c>
       <c r="I9" s="12">
@@ -1095,10 +1095,10 @@
       <c r="F12" s="8">
         <v>5</v>
       </c>
-      <c r="G12" s="10">
-        <v>5</v>
-      </c>
-      <c r="H12" s="10">
+      <c r="G12" s="8">
+        <v>5</v>
+      </c>
+      <c r="H12" s="8">
         <v>5</v>
       </c>
       <c r="I12" s="10">
@@ -1394,7 +1394,7 @@
       <c r="H17" s="8">
         <v>5</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="8">
         <v>5</v>
       </c>
       <c r="J17" s="7"/>
@@ -1490,13 +1490,13 @@
       <c r="F19" s="8">
         <v>5</v>
       </c>
-      <c r="G19" s="10">
-        <v>5</v>
-      </c>
-      <c r="H19" s="10">
-        <v>5</v>
-      </c>
-      <c r="I19" s="11" t="s">
+      <c r="G19" s="8">
+        <v>5</v>
+      </c>
+      <c r="H19" s="8">
+        <v>5</v>
+      </c>
+      <c r="I19" s="9" t="s">
         <v>37</v>
       </c>
       <c r="J19" s="7"/>
@@ -1538,13 +1538,13 @@
       <c r="C20" s="8">
         <v>5</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="8">
         <v>5</v>
       </c>
       <c r="E20" s="8">
         <v>5</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="9">
         <v>5</v>
       </c>
       <c r="G20" s="8">
@@ -1553,13 +1553,13 @@
       <c r="H20" s="8">
         <v>5</v>
       </c>
-      <c r="I20" s="10">
-        <v>5</v>
-      </c>
-      <c r="J20" s="7">
-        <v>5</v>
-      </c>
-      <c r="K20" s="11">
+      <c r="I20" s="8">
+        <v>5</v>
+      </c>
+      <c r="J20" s="9">
+        <v>5</v>
+      </c>
+      <c r="K20" s="9">
         <v>5</v>
       </c>
       <c r="L20" s="7">
@@ -1655,7 +1655,7 @@
       <c r="H22" s="8">
         <v>5</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="8">
         <v>5</v>
       </c>
       <c r="J22" s="7"/>
@@ -1712,13 +1712,13 @@
       <c r="H23" s="8">
         <v>5</v>
       </c>
-      <c r="I23" s="6">
-        <v>5</v>
-      </c>
-      <c r="J23" s="10">
-        <v>5</v>
-      </c>
-      <c r="K23" s="10">
+      <c r="I23" s="8">
+        <v>5</v>
+      </c>
+      <c r="J23" s="8">
+        <v>5</v>
+      </c>
+      <c r="K23" s="8">
         <v>5</v>
       </c>
       <c r="L23" s="11">
@@ -1830,13 +1830,13 @@
       <c r="H25" s="8">
         <v>5</v>
       </c>
-      <c r="I25" s="3">
-        <v>5</v>
-      </c>
-      <c r="J25" s="10">
-        <v>5</v>
-      </c>
-      <c r="K25" s="10">
+      <c r="I25" s="8">
+        <v>5</v>
+      </c>
+      <c r="J25" s="8">
+        <v>5</v>
+      </c>
+      <c r="K25" s="8">
         <v>5</v>
       </c>
       <c r="L25" s="7">
@@ -1887,19 +1887,19 @@
       <c r="F26" s="8">
         <v>5</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="8">
         <v>5</v>
       </c>
       <c r="H26" s="8">
         <v>5</v>
       </c>
-      <c r="I26" s="3">
-        <v>5</v>
-      </c>
-      <c r="J26" s="10">
-        <v>5</v>
-      </c>
-      <c r="K26" s="10">
+      <c r="I26" s="8">
+        <v>5</v>
+      </c>
+      <c r="J26" s="8">
+        <v>5</v>
+      </c>
+      <c r="K26" s="8">
         <v>5</v>
       </c>
       <c r="L26" s="11">
@@ -1956,13 +1956,13 @@
       <c r="H27" s="8">
         <v>5</v>
       </c>
-      <c r="I27" s="10">
-        <v>5</v>
-      </c>
-      <c r="J27" s="10">
-        <v>5</v>
-      </c>
-      <c r="K27" s="10">
+      <c r="I27" s="8">
+        <v>5</v>
+      </c>
+      <c r="J27" s="8">
+        <v>5</v>
+      </c>
+      <c r="K27" s="8">
         <v>5</v>
       </c>
       <c r="L27" s="12">
@@ -2053,7 +2053,7 @@
       <c r="H29" s="8">
         <v>5</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="8">
         <v>5</v>
       </c>
       <c r="J29" s="7"/>
@@ -2092,31 +2092,31 @@
       <c r="B30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="10">
-        <v>5</v>
-      </c>
-      <c r="D30" s="10">
-        <v>5</v>
-      </c>
-      <c r="E30" s="10">
-        <v>5</v>
-      </c>
-      <c r="F30" s="10">
-        <v>5</v>
-      </c>
-      <c r="G30" s="10">
-        <v>5</v>
-      </c>
-      <c r="H30" s="10">
-        <v>5</v>
-      </c>
-      <c r="I30" s="10">
-        <v>5</v>
-      </c>
-      <c r="J30" s="10">
-        <v>5</v>
-      </c>
-      <c r="K30" s="10">
+      <c r="C30" s="8">
+        <v>5</v>
+      </c>
+      <c r="D30" s="8">
+        <v>5</v>
+      </c>
+      <c r="E30" s="8">
+        <v>5</v>
+      </c>
+      <c r="F30" s="8">
+        <v>5</v>
+      </c>
+      <c r="G30" s="8">
+        <v>5</v>
+      </c>
+      <c r="H30" s="8">
+        <v>5</v>
+      </c>
+      <c r="I30" s="8">
+        <v>5</v>
+      </c>
+      <c r="J30" s="8">
+        <v>5</v>
+      </c>
+      <c r="K30" s="8">
         <v>5</v>
       </c>
       <c r="L30" s="7">
@@ -2173,14 +2173,14 @@
       <c r="H31" s="8">
         <v>5</v>
       </c>
-      <c r="I31" s="6">
-        <v>5</v>
-      </c>
-      <c r="J31" s="10">
-        <v>8</v>
-      </c>
-      <c r="K31" s="10">
-        <v>9</v>
+      <c r="I31" s="8">
+        <v>5</v>
+      </c>
+      <c r="J31" s="8">
+        <v>5</v>
+      </c>
+      <c r="K31" s="8">
+        <v>5</v>
       </c>
       <c r="L31" s="11">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 декабря 2023 г. 11:21:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -618,10 +618,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -707,12 +707,16 @@
     </row>
     <row r="4" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
+        <f>IF(B4=C4,1,"---")</f>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
@@ -723,19 +727,19 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4">
-        <f>IF($M4=N$2,1,0)</f>
+        <f t="shared" ref="N4:Q33" si="1">IF($M4=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O4" s="14">
-        <f>IF($M4=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4" s="14">
-        <f>IF($M4=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4" s="14">
-        <f>IF($M4=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R4" s="7"/>
@@ -747,6 +751,10 @@
     </row>
     <row r="5" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <f>IF(B5=C5,A4+1,"____")</f>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -771,25 +779,25 @@
         <v>5</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7">
         <v>2</v>
       </c>
       <c r="N5" s="14">
-        <f>IF($M5=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O5" s="14">
-        <f>IF($M5=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P5" s="14">
-        <f>IF($M5=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q5" s="14">
-        <f>IF($M5=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R5" s="7"/>
@@ -801,6 +809,10 @@
     </row>
     <row r="6" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
+        <f t="shared" ref="A6:A33" si="2">IF(B6=C6,A5+1,"____")</f>
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -819,19 +831,19 @@
         <v>1</v>
       </c>
       <c r="N6" s="14">
-        <f>IF($M6=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O6" s="14">
-        <f>IF($M6=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P6" s="14">
-        <f>IF($M6=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q6" s="14">
-        <f>IF($M6=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R6" s="7"/>
@@ -843,6 +855,10 @@
     </row>
     <row r="7" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -879,19 +895,19 @@
         <v>4</v>
       </c>
       <c r="N7" s="14">
-        <f>IF($M7=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O7" s="14">
-        <f>IF($M7=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7" s="14">
-        <f>IF($M7=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q7" s="14">
-        <f>IF($M7=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R7" s="7"/>
@@ -905,6 +921,10 @@
     </row>
     <row r="8" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -941,19 +961,19 @@
         <v>1</v>
       </c>
       <c r="N8" s="14">
-        <f>IF($M8=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O8" s="14">
-        <f>IF($M8=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P8" s="14">
-        <f>IF($M8=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q8" s="14">
-        <f>IF($M8=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R8" s="7"/>
@@ -965,6 +985,10 @@
     </row>
     <row r="9" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1001,19 +1025,19 @@
         <v>1</v>
       </c>
       <c r="N9" s="14">
-        <f>IF($M9=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O9" s="14">
-        <f>IF($M9=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P9" s="14">
-        <f>IF($M9=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q9" s="14">
-        <f>IF($M9=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R9" s="7"/>
@@ -1025,6 +1049,10 @@
     </row>
     <row r="10" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1041,19 +1069,19 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="14">
-        <f>IF($M10=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O10" s="14">
-        <f>IF($M10=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P10" s="14">
-        <f>IF($M10=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q10" s="14">
-        <f>IF($M10=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R10" s="7"/>
@@ -1065,6 +1093,10 @@
     </row>
     <row r="11" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1101,19 +1133,19 @@
         <v>2</v>
       </c>
       <c r="N11" s="14">
-        <f>IF($M11=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O11" s="14">
-        <f>IF($M11=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P11" s="14">
-        <f>IF($M11=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q11" s="14">
-        <f>IF($M11=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R11" s="7"/>
@@ -1127,6 +1159,10 @@
     </row>
     <row r="12" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1163,19 +1199,19 @@
         <v>4</v>
       </c>
       <c r="N12" s="14">
-        <f>IF($M12=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O12" s="14">
-        <f>IF($M12=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P12" s="14">
-        <f>IF($M12=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q12" s="14">
-        <f>IF($M12=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R12" s="7"/>
@@ -1189,6 +1225,10 @@
     </row>
     <row r="13" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1225,19 +1265,19 @@
         <v>3</v>
       </c>
       <c r="N13" s="14">
-        <f>IF($M13=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O13" s="14">
-        <f>IF($M13=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P13" s="14">
-        <f>IF($M13=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q13" s="14">
-        <f>IF($M13=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R13" s="7"/>
@@ -1251,6 +1291,10 @@
     </row>
     <row r="14" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1287,19 +1331,19 @@
         <v>3</v>
       </c>
       <c r="N14" s="14">
-        <f>IF($M14=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O14" s="14">
-        <f>IF($M14=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P14" s="14">
-        <f>IF($M14=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q14" s="14">
-        <f>IF($M14=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="7"/>
@@ -1311,6 +1355,10 @@
     </row>
     <row r="15" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1329,19 +1377,19 @@
         <v>4</v>
       </c>
       <c r="N15" s="14">
-        <f>IF($M15=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O15" s="14">
-        <f>IF($M15=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P15" s="14">
-        <f>IF($M15=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q15" s="14">
-        <f>IF($M15=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R15" s="7"/>
@@ -1353,6 +1401,10 @@
     </row>
     <row r="16" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1389,19 +1441,19 @@
         <v>4</v>
       </c>
       <c r="N16" s="14">
-        <f>IF($M16=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O16" s="14">
-        <f>IF($M16=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" s="14">
-        <f>IF($M16=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q16" s="14">
-        <f>IF($M16=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R16" s="7"/>
@@ -1415,6 +1467,10 @@
     </row>
     <row r="17" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1435,19 +1491,19 @@
         <v>2</v>
       </c>
       <c r="N17" s="14">
-        <f>IF($M17=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O17" s="14">
-        <f>IF($M17=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P17" s="14">
-        <f>IF($M17=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q17" s="14">
-        <f>IF($M17=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R17" s="7"/>
@@ -1459,6 +1515,10 @@
     </row>
     <row r="18" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1491,19 +1551,19 @@
         <v>1</v>
       </c>
       <c r="N18" s="14">
-        <f>IF($M18=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O18" s="14">
-        <f>IF($M18=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P18" s="14">
-        <f>IF($M18=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q18" s="14">
-        <f>IF($M18=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R18" s="7"/>
@@ -1515,6 +1575,10 @@
     </row>
     <row r="19" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1551,19 +1615,19 @@
         <v>4</v>
       </c>
       <c r="N19" s="14">
-        <f>IF($M19=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O19" s="14">
-        <f>IF($M19=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P19" s="14">
-        <f>IF($M19=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q19" s="14">
-        <f>IF($M19=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R19" s="7"/>
@@ -1575,6 +1639,10 @@
     </row>
     <row r="20" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1593,19 +1661,19 @@
         <v>3</v>
       </c>
       <c r="N20" s="14">
-        <f>IF($M20=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O20" s="14">
-        <f>IF($M20=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20" s="14">
-        <f>IF($M20=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q20" s="14">
-        <f>IF($M20=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R20" s="7"/>
@@ -1617,6 +1685,10 @@
     </row>
     <row r="21" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1647,19 +1719,19 @@
         <v>3</v>
       </c>
       <c r="N21" s="14">
-        <f>IF($M21=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O21" s="14">
-        <f>IF($M21=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21" s="14">
-        <f>IF($M21=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q21" s="14">
-        <f>IF($M21=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21" s="7"/>
@@ -1671,7 +1743,11 @@
     </row>
     <row r="22" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
+        <f t="shared" si="2"/>
         <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>33</v>
@@ -1707,19 +1783,19 @@
         <v>3</v>
       </c>
       <c r="N22" s="14">
-        <f>IF($M22=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O22" s="14">
-        <f>IF($M22=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P22" s="14">
-        <f>IF($M22=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q22" s="14">
-        <f>IF($M22=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R22" s="7"/>
@@ -1733,7 +1809,11 @@
     </row>
     <row r="23" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
+        <f t="shared" si="2"/>
         <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
@@ -1763,19 +1843,19 @@
         <v>1</v>
       </c>
       <c r="N23" s="14">
-        <f>IF($M23=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O23" s="14">
-        <f>IF($M23=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P23" s="14">
-        <f>IF($M23=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q23" s="14">
-        <f>IF($M23=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R23" s="7"/>
@@ -1787,7 +1867,11 @@
     </row>
     <row r="24" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
+        <f t="shared" si="2"/>
         <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -1823,19 +1907,19 @@
         <v>1</v>
       </c>
       <c r="N24" s="14">
-        <f>IF($M24=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O24" s="14">
-        <f>IF($M24=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P24" s="14">
-        <f>IF($M24=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q24" s="14">
-        <f>IF($M24=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R24" s="7"/>
@@ -1849,7 +1933,11 @@
     </row>
     <row r="25" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
+        <f t="shared" si="2"/>
         <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>21</v>
@@ -1885,19 +1973,19 @@
         <v>4</v>
       </c>
       <c r="N25" s="14">
-        <f>IF($M25=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O25" s="14">
-        <f>IF($M25=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P25" s="14">
-        <f>IF($M25=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q25" s="14">
-        <f>IF($M25=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R25" s="7"/>
@@ -1911,7 +1999,11 @@
     </row>
     <row r="26" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
+        <f t="shared" si="2"/>
         <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>22</v>
@@ -1947,19 +2039,19 @@
         <v>4</v>
       </c>
       <c r="N26" s="14">
-        <f>IF($M26=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O26" s="14">
-        <f>IF($M26=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P26" s="14">
-        <f>IF($M26=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q26" s="14">
-        <f>IF($M26=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R26" s="7"/>
@@ -1973,7 +2065,11 @@
     </row>
     <row r="27" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
+        <f t="shared" si="2"/>
         <v>24</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>38</v>
@@ -1982,19 +2078,19 @@
         <v>2</v>
       </c>
       <c r="N27" s="17">
-        <f>IF($M27=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O27" s="17">
-        <f>IF($M27=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P27" s="17">
-        <f>IF($M27=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q27" s="17">
-        <f>IF($M27=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R27" s="7"/>
@@ -2006,7 +2102,11 @@
     </row>
     <row r="28" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
+        <f t="shared" si="2"/>
         <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>23</v>
@@ -2038,19 +2138,19 @@
         <v>1</v>
       </c>
       <c r="N28" s="14">
-        <f>IF($M28=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O28" s="14">
-        <f>IF($M28=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P28" s="14">
-        <f>IF($M28=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q28" s="14">
-        <f>IF($M28=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="7"/>
@@ -2062,7 +2162,11 @@
     </row>
     <row r="29" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
+        <f t="shared" si="2"/>
         <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>24</v>
@@ -2098,19 +2202,19 @@
         <v>2</v>
       </c>
       <c r="N29" s="14">
-        <f>IF($M29=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O29" s="14">
-        <f>IF($M29=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P29" s="14">
-        <f>IF($M29=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q29" s="14">
-        <f>IF($M29=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="7"/>
@@ -2124,7 +2228,11 @@
     </row>
     <row r="30" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
+        <f t="shared" si="2"/>
         <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>25</v>
@@ -2160,19 +2268,19 @@
         <v>3</v>
       </c>
       <c r="N30" s="14">
-        <f>IF($M30=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O30" s="14">
-        <f>IF($M30=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P30" s="14">
-        <f>IF($M30=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q30" s="14">
-        <f>IF($M30=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="7"/>
@@ -2186,7 +2294,11 @@
     </row>
     <row r="31" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
+        <f t="shared" si="2"/>
         <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>26</v>
@@ -2216,19 +2328,19 @@
         <v>3</v>
       </c>
       <c r="N31" s="14">
-        <f>IF($M31=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O31" s="14">
-        <f>IF($M31=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P31" s="14">
-        <f>IF($M31=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q31" s="14">
-        <f>IF($M31=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R31" s="7"/>
@@ -2240,7 +2352,11 @@
     </row>
     <row r="32" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
+        <f t="shared" si="2"/>
         <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>27</v>
@@ -2266,19 +2382,19 @@
         <v>2</v>
       </c>
       <c r="N32" s="14">
-        <f>IF($M32=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O32" s="14">
-        <f>IF($M32=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P32" s="14">
-        <f>IF($M32=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q32" s="14">
-        <f>IF($M32=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R32" s="7"/>
@@ -2290,7 +2406,11 @@
     </row>
     <row r="33" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
+        <f t="shared" si="2"/>
         <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>28</v>
@@ -2314,19 +2434,19 @@
         <v>2</v>
       </c>
       <c r="N33" s="14">
-        <f>IF($M33=N$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O33" s="14">
-        <f>IF($M33=O$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P33" s="14">
-        <f>IF($M33=P$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q33" s="14">
-        <f>IF($M33=Q$2,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R33" s="7"/>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 10:58:30_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -643,7 +643,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
       </c>
       <c r="P3" s="10">
         <f>SUM(P4:P35)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q3" s="10">
         <f>SUM(Q4:Q35)</f>
@@ -1082,17 +1082,19 @@
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="9">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="6">
+        <v>3</v>
+      </c>
+      <c r="N10" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1102,7 +1104,7 @@
       </c>
       <c r="P10" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="9">
         <f t="shared" si="0"/>
@@ -1371,7 +1373,9 @@
         <v>0</v>
       </c>
       <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
+      <c r="S14" s="7">
+        <v>5</v>
+      </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
@@ -1503,14 +1507,30 @@
       <c r="D17" s="20">
         <v>5</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
+      <c r="E17" s="17">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17">
+        <v>5</v>
+      </c>
+      <c r="G17" s="17">
+        <v>5</v>
+      </c>
+      <c r="H17" s="17">
+        <v>5</v>
+      </c>
+      <c r="I17" s="17">
+        <v>5</v>
+      </c>
+      <c r="J17" s="17">
+        <v>5</v>
+      </c>
+      <c r="K17" s="17">
+        <v>5</v>
+      </c>
+      <c r="L17" s="17">
+        <v>5</v>
+      </c>
       <c r="M17" s="6">
         <v>2</v>
       </c>
@@ -1569,8 +1589,12 @@
       <c r="J18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
+      <c r="K18" s="17">
+        <v>5</v>
+      </c>
+      <c r="L18" s="17">
+        <v>5</v>
+      </c>
       <c r="M18" s="6">
         <v>1</v>
       </c>
@@ -1591,7 +1615,9 @@
         <v>0</v>
       </c>
       <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
+      <c r="S18" s="4">
+        <v>5</v>
+      </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
@@ -1721,7 +1747,7 @@
       <c r="D21" s="20">
         <v>5</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="20">
         <v>5</v>
       </c>
@@ -1737,8 +1763,12 @@
       <c r="J21" s="25">
         <v>5</v>
       </c>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
+      <c r="K21" s="3">
+        <v>5</v>
+      </c>
+      <c r="L21" s="3">
+        <v>5</v>
+      </c>
       <c r="M21" s="6">
         <v>3</v>
       </c>
@@ -1759,7 +1789,9 @@
         <v>0</v>
       </c>
       <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
+      <c r="S21" s="4">
+        <v>5</v>
+      </c>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
@@ -2454,15 +2486,27 @@
       <c r="E33" s="20">
         <v>5</v>
       </c>
-      <c r="F33" s="20"/>
+      <c r="F33" s="3">
+        <v>5</v>
+      </c>
       <c r="G33" s="20">
         <v>5</v>
       </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
+      <c r="H33" s="3">
+        <v>5</v>
+      </c>
+      <c r="I33" s="3">
+        <v>5</v>
+      </c>
+      <c r="J33" s="3">
+        <v>5</v>
+      </c>
+      <c r="K33" s="3">
+        <v>5</v>
+      </c>
+      <c r="L33" s="3">
+        <v>5</v>
+      </c>
       <c r="M33" s="6">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 11:51:16_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -640,10 +640,10 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1001,9 @@
         <v>0</v>
       </c>
       <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="S8" s="4">
+        <v>5</v>
+      </c>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -1551,7 +1553,9 @@
         <v>0</v>
       </c>
       <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
+      <c r="S17" s="7">
+        <v>5</v>
+      </c>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
@@ -1681,7 +1685,9 @@
         <v>1</v>
       </c>
       <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
+      <c r="S19" s="7">
+        <v>5</v>
+      </c>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
@@ -1892,9 +1898,15 @@
       <c r="I23" s="20">
         <v>5</v>
       </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
+      <c r="J23" s="6">
+        <v>5</v>
+      </c>
+      <c r="K23" s="6">
+        <v>5</v>
+      </c>
+      <c r="L23" s="6">
+        <v>5</v>
+      </c>
       <c r="M23" s="6">
         <v>1</v>
       </c>
@@ -1915,7 +1927,9 @@
         <v>0</v>
       </c>
       <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
+      <c r="S23" s="7">
+        <v>5</v>
+      </c>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
@@ -2429,20 +2443,30 @@
       <c r="D32" s="20">
         <v>5</v>
       </c>
-      <c r="E32" s="20"/>
+      <c r="E32" s="5">
+        <v>5</v>
+      </c>
       <c r="F32" s="20">
         <v>5</v>
       </c>
-      <c r="G32" s="23"/>
+      <c r="G32" s="17">
+        <v>5</v>
+      </c>
       <c r="H32" s="20">
         <v>5</v>
       </c>
       <c r="I32" s="20">
         <v>5</v>
       </c>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
+      <c r="J32" s="17">
+        <v>5</v>
+      </c>
+      <c r="K32" s="17">
+        <v>5</v>
+      </c>
+      <c r="L32" s="17">
+        <v>5</v>
+      </c>
       <c r="M32" s="6">
         <v>2</v>
       </c>
@@ -2463,7 +2487,9 @@
         <v>0</v>
       </c>
       <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
+      <c r="S32" s="4">
+        <v>5</v>
+      </c>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
@@ -2527,7 +2553,9 @@
         <v>0</v>
       </c>
       <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
+      <c r="S33" s="7">
+        <v>5</v>
+      </c>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 10:15:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -640,10 +640,10 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
+      <selection pane="bottomRight" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2211,8 +2211,12 @@
       <c r="J28" s="25">
         <v>5</v>
       </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
+      <c r="K28" s="17">
+        <v>5</v>
+      </c>
+      <c r="L28" s="17">
+        <v>5</v>
+      </c>
       <c r="M28" s="6">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 10:42:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -640,10 +640,10 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S28" sqref="S28"/>
+      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,9 @@
         <v>0</v>
       </c>
       <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="S9" s="4">
+        <v>5</v>
+      </c>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 11:53:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -181,6 +181,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -318,15 +324,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -637,13 +643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
+      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -740,13 +746,13 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="24"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -802,9 +808,9 @@
       <c r="I5" s="20">
         <v>5</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="6">
         <v>2</v>
       </c>
@@ -842,15 +848,33 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>5</v>
+      </c>
+      <c r="K6" s="6">
+        <v>5</v>
+      </c>
+      <c r="L6" s="6">
+        <v>5</v>
+      </c>
       <c r="M6" s="6">
         <v>1</v>
       </c>
@@ -871,7 +895,9 @@
         <v>0</v>
       </c>
       <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="S6" s="4">
+        <v>5</v>
+      </c>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -906,13 +932,13 @@
       <c r="I7" s="20">
         <v>5</v>
       </c>
-      <c r="J7" s="25">
-        <v>5</v>
-      </c>
-      <c r="K7" s="25">
-        <v>5</v>
-      </c>
-      <c r="L7" s="25">
+      <c r="J7" s="23">
+        <v>5</v>
+      </c>
+      <c r="K7" s="23">
+        <v>5</v>
+      </c>
+      <c r="L7" s="23">
         <v>5</v>
       </c>
       <c r="M7" s="6">
@@ -963,22 +989,22 @@
       <c r="F8" s="20">
         <v>5</v>
       </c>
-      <c r="G8" s="23">
-        <v>5</v>
-      </c>
-      <c r="H8" s="23">
-        <v>5</v>
-      </c>
-      <c r="I8" s="23">
-        <v>5</v>
-      </c>
-      <c r="J8" s="24">
-        <v>5</v>
-      </c>
-      <c r="K8" s="24">
-        <v>5</v>
-      </c>
-      <c r="L8" s="24">
+      <c r="G8" s="21">
+        <v>5</v>
+      </c>
+      <c r="H8" s="21">
+        <v>5</v>
+      </c>
+      <c r="I8" s="21">
+        <v>5</v>
+      </c>
+      <c r="J8" s="22">
+        <v>5</v>
+      </c>
+      <c r="K8" s="22">
+        <v>5</v>
+      </c>
+      <c r="L8" s="22">
         <v>4</v>
       </c>
       <c r="M8" s="6">
@@ -1038,13 +1064,13 @@
       <c r="I9" s="20">
         <v>5</v>
       </c>
-      <c r="J9" s="25">
-        <v>5</v>
-      </c>
-      <c r="K9" s="25">
-        <v>5</v>
-      </c>
-      <c r="L9" s="25">
+      <c r="J9" s="23">
+        <v>5</v>
+      </c>
+      <c r="K9" s="23">
+        <v>5</v>
+      </c>
+      <c r="L9" s="23">
         <v>5</v>
       </c>
       <c r="M9" s="6">
@@ -1150,13 +1176,13 @@
       <c r="I11" s="20">
         <v>5</v>
       </c>
-      <c r="J11" s="25">
-        <v>5</v>
-      </c>
-      <c r="K11" s="25">
-        <v>5</v>
-      </c>
-      <c r="L11" s="25">
+      <c r="J11" s="23">
+        <v>5</v>
+      </c>
+      <c r="K11" s="23">
+        <v>5</v>
+      </c>
+      <c r="L11" s="23">
         <v>5</v>
       </c>
       <c r="M11" s="6">
@@ -1216,13 +1242,13 @@
       <c r="I12" s="20">
         <v>5</v>
       </c>
-      <c r="J12" s="25">
-        <v>5</v>
-      </c>
-      <c r="K12" s="25">
-        <v>5</v>
-      </c>
-      <c r="L12" s="25">
+      <c r="J12" s="23">
+        <v>5</v>
+      </c>
+      <c r="K12" s="23">
+        <v>5</v>
+      </c>
+      <c r="L12" s="23">
         <v>5</v>
       </c>
       <c r="M12" s="6">
@@ -1282,13 +1308,13 @@
       <c r="I13" s="20">
         <v>5</v>
       </c>
-      <c r="J13" s="25">
-        <v>5</v>
-      </c>
-      <c r="K13" s="25">
-        <v>5</v>
-      </c>
-      <c r="L13" s="25">
+      <c r="J13" s="23">
+        <v>5</v>
+      </c>
+      <c r="K13" s="23">
+        <v>5</v>
+      </c>
+      <c r="L13" s="23">
         <v>5</v>
       </c>
       <c r="M13" s="6">
@@ -1348,13 +1374,13 @@
       <c r="I14" s="20">
         <v>5</v>
       </c>
-      <c r="J14" s="25">
-        <v>5</v>
-      </c>
-      <c r="K14" s="25">
-        <v>5</v>
-      </c>
-      <c r="L14" s="25">
+      <c r="J14" s="23">
+        <v>5</v>
+      </c>
+      <c r="K14" s="23">
+        <v>5</v>
+      </c>
+      <c r="L14" s="23">
         <v>5</v>
       </c>
       <c r="M14" s="6">
@@ -1399,12 +1425,12 @@
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
       <c r="M15" s="6">
         <v>4</v>
       </c>
@@ -1460,13 +1486,13 @@
       <c r="I16" s="20">
         <v>5</v>
       </c>
-      <c r="J16" s="25">
-        <v>5</v>
-      </c>
-      <c r="K16" s="25">
-        <v>5</v>
-      </c>
-      <c r="L16" s="25">
+      <c r="J16" s="23">
+        <v>5</v>
+      </c>
+      <c r="K16" s="23">
+        <v>5</v>
+      </c>
+      <c r="L16" s="23">
         <v>5</v>
       </c>
       <c r="M16" s="6">
@@ -1592,7 +1618,7 @@
       <c r="I18" s="20">
         <v>5</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="22" t="s">
         <v>37</v>
       </c>
       <c r="K18" s="17">
@@ -1649,7 +1675,7 @@
       <c r="F19" s="20">
         <v>5</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="21">
         <v>5</v>
       </c>
       <c r="H19" s="20">
@@ -1658,13 +1684,13 @@
       <c r="I19" s="20">
         <v>5</v>
       </c>
-      <c r="J19" s="25">
-        <v>5</v>
-      </c>
-      <c r="K19" s="24">
-        <v>5</v>
-      </c>
-      <c r="L19" s="24">
+      <c r="J19" s="23">
+        <v>5</v>
+      </c>
+      <c r="K19" s="22">
+        <v>5</v>
+      </c>
+      <c r="L19" s="22">
         <v>5</v>
       </c>
       <c r="M19" s="6">
@@ -1706,15 +1732,33 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
+      <c r="D20" s="24">
+        <v>5</v>
+      </c>
+      <c r="E20" s="25">
+        <v>5</v>
+      </c>
+      <c r="F20" s="25">
+        <v>5</v>
+      </c>
+      <c r="G20" s="25">
+        <v>5</v>
+      </c>
+      <c r="H20" s="25">
+        <v>5</v>
+      </c>
+      <c r="I20" s="25">
+        <v>5</v>
+      </c>
+      <c r="J20" s="25">
+        <v>5</v>
+      </c>
+      <c r="K20" s="25">
+        <v>5</v>
+      </c>
+      <c r="L20" s="25">
+        <v>5</v>
+      </c>
       <c r="M20" s="6">
         <v>3</v>
       </c>
@@ -1735,7 +1779,9 @@
         <v>0</v>
       </c>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+      <c r="S20" s="7">
+        <v>5</v>
+      </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
@@ -1768,7 +1814,7 @@
       <c r="I21" s="20">
         <v>5</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21" s="23">
         <v>5</v>
       </c>
       <c r="K21" s="3">
@@ -1834,13 +1880,13 @@
       <c r="I22" s="20">
         <v>5</v>
       </c>
-      <c r="J22" s="25">
-        <v>5</v>
-      </c>
-      <c r="K22" s="25">
-        <v>5</v>
-      </c>
-      <c r="L22" s="25">
+      <c r="J22" s="23">
+        <v>5</v>
+      </c>
+      <c r="K22" s="23">
+        <v>5</v>
+      </c>
+      <c r="L22" s="23">
         <v>5</v>
       </c>
       <c r="M22" s="6">
@@ -1966,13 +2012,13 @@
       <c r="I24" s="20">
         <v>5</v>
       </c>
-      <c r="J24" s="25">
-        <v>5</v>
-      </c>
-      <c r="K24" s="25">
-        <v>5</v>
-      </c>
-      <c r="L24" s="25">
+      <c r="J24" s="23">
+        <v>5</v>
+      </c>
+      <c r="K24" s="23">
+        <v>5</v>
+      </c>
+      <c r="L24" s="23">
         <v>5</v>
       </c>
       <c r="M24" s="6">
@@ -2032,13 +2078,13 @@
       <c r="I25" s="20">
         <v>5</v>
       </c>
-      <c r="J25" s="25">
-        <v>5</v>
-      </c>
-      <c r="K25" s="25">
-        <v>5</v>
-      </c>
-      <c r="L25" s="25">
+      <c r="J25" s="23">
+        <v>5</v>
+      </c>
+      <c r="K25" s="23">
+        <v>5</v>
+      </c>
+      <c r="L25" s="23">
         <v>5</v>
       </c>
       <c r="M25" s="6">
@@ -2098,13 +2144,13 @@
       <c r="I26" s="20">
         <v>5</v>
       </c>
-      <c r="J26" s="25">
-        <v>5</v>
-      </c>
-      <c r="K26" s="25">
-        <v>5</v>
-      </c>
-      <c r="L26" s="25">
+      <c r="J26" s="23">
+        <v>5</v>
+      </c>
+      <c r="K26" s="23">
+        <v>5</v>
+      </c>
+      <c r="L26" s="23">
         <v>5</v>
       </c>
       <c r="M26" s="6">
@@ -2146,15 +2192,14 @@
       <c r="C27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
       <c r="M27" s="6">
         <v>2</v>
       </c>
@@ -2210,7 +2255,7 @@
       <c r="I28" s="20">
         <v>5</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="23">
         <v>5</v>
       </c>
       <c r="K28" s="17">
@@ -2239,7 +2284,9 @@
         <v>0</v>
       </c>
       <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
+      <c r="S28" s="7">
+        <v>5</v>
+      </c>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
@@ -2274,13 +2321,13 @@
       <c r="I29" s="20">
         <v>5</v>
       </c>
-      <c r="J29" s="25">
-        <v>5</v>
-      </c>
-      <c r="K29" s="25">
-        <v>5</v>
-      </c>
-      <c r="L29" s="25">
+      <c r="J29" s="23">
+        <v>5</v>
+      </c>
+      <c r="K29" s="23">
+        <v>5</v>
+      </c>
+      <c r="L29" s="23">
         <v>5</v>
       </c>
       <c r="M29" s="6">
@@ -2331,7 +2378,7 @@
       <c r="F30" s="20">
         <v>5</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="21">
         <v>5</v>
       </c>
       <c r="H30" s="20">
@@ -2340,13 +2387,13 @@
       <c r="I30" s="20">
         <v>5</v>
       </c>
-      <c r="J30" s="25">
-        <v>5</v>
-      </c>
-      <c r="K30" s="25">
-        <v>5</v>
-      </c>
-      <c r="L30" s="25">
+      <c r="J30" s="23">
+        <v>5</v>
+      </c>
+      <c r="K30" s="23">
+        <v>5</v>
+      </c>
+      <c r="L30" s="23">
         <v>5</v>
       </c>
       <c r="M30" s="6">
@@ -2406,9 +2453,9 @@
       <c r="I31" s="20">
         <v>5</v>
       </c>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
       <c r="M31" s="6">
         <v>3</v>
       </c>
@@ -2571,11 +2618,11 @@
       <c r="D34" s="18">
         <v>1</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
@@ -2586,7 +2633,7 @@
       <c r="Q34" s="9"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E35" s="21"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
@@ -2601,7 +2648,7 @@
       <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E36" s="21"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -2612,7 +2659,7 @@
       <c r="M36" s="17"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E37" s="21"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
@@ -2623,7 +2670,7 @@
       <c r="M37" s="17"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E38" s="21"/>
+      <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -2634,7 +2681,7 @@
       <c r="M38" s="17"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E39" s="21"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
@@ -2645,7 +2692,7 @@
       <c r="M39" s="17"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E40" s="21"/>
+      <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
       <c r="H40" s="17"/>
@@ -2656,7 +2703,7 @@
       <c r="M40" s="17"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E41" s="21"/>
+      <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
       <c r="H41" s="17"/>
@@ -2667,7 +2714,7 @@
       <c r="M41" s="17"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E42" s="21"/>
+      <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
@@ -2678,7 +2725,7 @@
       <c r="M42" s="17"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E43" s="21"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
@@ -2689,10 +2736,44 @@
       <c r="M43" s="17"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
       <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
       <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 15:05:04_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -646,10 +646,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2453,9 +2453,9 @@
       <c r="I31" s="20">
         <v>5</v>
       </c>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
       <c r="M31" s="6">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_20 декабря 2023 г. 10:47:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -646,10 +646,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31:L31"/>
+      <selection pane="bottomRight" activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1422,15 +1422,15 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
       <c r="M15" s="6">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 13:08:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -646,10 +646,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S27" sqref="S27"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1112,15 +1112,33 @@
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5">
+        <v>5</v>
+      </c>
+      <c r="I10" s="5">
+        <v>5</v>
+      </c>
+      <c r="J10" s="5">
+        <v>5</v>
+      </c>
+      <c r="K10" s="5">
+        <v>5</v>
+      </c>
+      <c r="L10" s="5">
+        <v>5</v>
+      </c>
       <c r="M10" s="6">
         <v>3</v>
       </c>
@@ -1422,14 +1440,30 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5</v>
+      </c>
+      <c r="G15" s="6">
+        <v>5</v>
+      </c>
+      <c r="H15" s="6">
+        <v>5</v>
+      </c>
+      <c r="I15" s="6">
+        <v>5</v>
+      </c>
+      <c r="J15" s="6">
+        <v>5</v>
+      </c>
+      <c r="K15" s="6">
+        <v>5</v>
+      </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6">
         <v>4</v>
@@ -2220,7 +2254,9 @@
         <v>0</v>
       </c>
       <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
+      <c r="S27" s="7">
+        <v>3</v>
+      </c>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 13:46:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -646,10 +646,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1159,9 @@
         <v>0</v>
       </c>
       <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
+      <c r="S10" s="7">
+        <v>5</v>
+      </c>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -1485,7 +1487,9 @@
         <v>1</v>
       </c>
       <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="S15" s="7">
+        <v>5</v>
+      </c>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 14:15:36_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Оценки ДифЗачет</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>авансом</t>
   </si>
 </sst>
 </file>
@@ -646,10 +652,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomRight" activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -773,7 +779,9 @@
         <v>0</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="S4" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
@@ -831,8 +839,12 @@
         <v>0</v>
       </c>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
+      <c r="S5" s="4">
+        <v>4</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
@@ -2516,8 +2528,12 @@
         <v>0</v>
       </c>
       <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
+      <c r="S31" s="7">
+        <v>5</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_21 декабря 2023 г. 15:08:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ДисМат_.xlsx
+++ b/2ИСИП-122_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -170,11 +170,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -198,7 +193,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +215,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF09C39F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -314,8 +315,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -323,9 +324,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -335,10 +333,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -652,10 +658,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T33" sqref="T33"/>
+      <selection pane="bottomRight" activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -668,7 +674,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C1" s="19"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
@@ -730,7 +736,7 @@
       </c>
       <c r="O3" s="10">
         <f>SUM(O4:O35)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P3" s="10">
         <f>SUM(P4:P35)</f>
@@ -763,7 +769,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4">
-        <f t="shared" ref="N4:Q33" si="0">IF($M4=N$2,1,0)</f>
+        <f t="shared" ref="N4:Q45" si="0">IF($M4=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O4" s="9">
@@ -798,22 +804,22 @@
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="20">
-        <v>5</v>
-      </c>
-      <c r="E5" s="20">
-        <v>5</v>
-      </c>
-      <c r="F5" s="20">
-        <v>5</v>
-      </c>
-      <c r="G5" s="20">
-        <v>5</v>
-      </c>
-      <c r="H5" s="20">
-        <v>5</v>
-      </c>
-      <c r="I5" s="20">
+      <c r="D5" s="19">
+        <v>5</v>
+      </c>
+      <c r="E5" s="19">
+        <v>5</v>
+      </c>
+      <c r="F5" s="19">
+        <v>5</v>
+      </c>
+      <c r="G5" s="19">
+        <v>5</v>
+      </c>
+      <c r="H5" s="19">
+        <v>5</v>
+      </c>
+      <c r="I5" s="19">
         <v>5</v>
       </c>
       <c r="J5" s="6"/>
@@ -860,31 +866,31 @@
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6">
-        <v>5</v>
-      </c>
-      <c r="H6" s="6">
-        <v>5</v>
-      </c>
-      <c r="I6" s="6">
-        <v>5</v>
-      </c>
-      <c r="J6" s="6">
-        <v>5</v>
-      </c>
-      <c r="K6" s="6">
-        <v>5</v>
-      </c>
-      <c r="L6" s="6">
+      <c r="D6" s="23">
+        <v>5</v>
+      </c>
+      <c r="E6" s="23">
+        <v>5</v>
+      </c>
+      <c r="F6" s="23">
+        <v>5</v>
+      </c>
+      <c r="G6" s="24">
+        <v>5</v>
+      </c>
+      <c r="H6" s="24">
+        <v>5</v>
+      </c>
+      <c r="I6" s="24">
+        <v>5</v>
+      </c>
+      <c r="J6" s="24">
+        <v>5</v>
+      </c>
+      <c r="K6" s="24">
+        <v>5</v>
+      </c>
+      <c r="L6" s="24">
         <v>5</v>
       </c>
       <c r="M6" s="6">
@@ -926,31 +932,31 @@
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="20">
-        <v>5</v>
-      </c>
-      <c r="E7" s="20">
-        <v>5</v>
-      </c>
-      <c r="F7" s="20">
-        <v>5</v>
-      </c>
-      <c r="G7" s="20">
-        <v>5</v>
-      </c>
-      <c r="H7" s="20">
-        <v>5</v>
-      </c>
-      <c r="I7" s="20">
-        <v>5</v>
-      </c>
-      <c r="J7" s="23">
-        <v>5</v>
-      </c>
-      <c r="K7" s="23">
-        <v>5</v>
-      </c>
-      <c r="L7" s="23">
+      <c r="D7" s="19">
+        <v>5</v>
+      </c>
+      <c r="E7" s="19">
+        <v>5</v>
+      </c>
+      <c r="F7" s="19">
+        <v>5</v>
+      </c>
+      <c r="G7" s="19">
+        <v>5</v>
+      </c>
+      <c r="H7" s="19">
+        <v>5</v>
+      </c>
+      <c r="I7" s="19">
+        <v>5</v>
+      </c>
+      <c r="J7" s="22">
+        <v>5</v>
+      </c>
+      <c r="K7" s="22">
+        <v>5</v>
+      </c>
+      <c r="L7" s="22">
         <v>5</v>
       </c>
       <c r="M7" s="6">
@@ -992,31 +998,31 @@
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="20">
-        <v>5</v>
-      </c>
-      <c r="E8" s="20">
-        <v>5</v>
-      </c>
-      <c r="F8" s="20">
-        <v>5</v>
-      </c>
-      <c r="G8" s="21">
-        <v>5</v>
-      </c>
-      <c r="H8" s="21">
-        <v>5</v>
-      </c>
-      <c r="I8" s="21">
-        <v>5</v>
-      </c>
-      <c r="J8" s="22">
-        <v>5</v>
-      </c>
-      <c r="K8" s="22">
-        <v>5</v>
-      </c>
-      <c r="L8" s="22">
+      <c r="D8" s="19">
+        <v>5</v>
+      </c>
+      <c r="E8" s="19">
+        <v>5</v>
+      </c>
+      <c r="F8" s="19">
+        <v>5</v>
+      </c>
+      <c r="G8" s="20">
+        <v>5</v>
+      </c>
+      <c r="H8" s="20">
+        <v>5</v>
+      </c>
+      <c r="I8" s="20">
+        <v>5</v>
+      </c>
+      <c r="J8" s="21">
+        <v>5</v>
+      </c>
+      <c r="K8" s="21">
+        <v>5</v>
+      </c>
+      <c r="L8" s="21">
         <v>4</v>
       </c>
       <c r="M8" s="6">
@@ -1058,31 +1064,31 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="20">
-        <v>5</v>
-      </c>
-      <c r="E9" s="20">
-        <v>5</v>
-      </c>
-      <c r="F9" s="20">
-        <v>5</v>
-      </c>
-      <c r="G9" s="20">
-        <v>5</v>
-      </c>
-      <c r="H9" s="20">
-        <v>5</v>
-      </c>
-      <c r="I9" s="20">
-        <v>5</v>
-      </c>
-      <c r="J9" s="23">
-        <v>5</v>
-      </c>
-      <c r="K9" s="23">
-        <v>5</v>
-      </c>
-      <c r="L9" s="23">
+      <c r="D9" s="19">
+        <v>5</v>
+      </c>
+      <c r="E9" s="19">
+        <v>5</v>
+      </c>
+      <c r="F9" s="19">
+        <v>5</v>
+      </c>
+      <c r="G9" s="19">
+        <v>5</v>
+      </c>
+      <c r="H9" s="19">
+        <v>5</v>
+      </c>
+      <c r="I9" s="19">
+        <v>5</v>
+      </c>
+      <c r="J9" s="22">
+        <v>5</v>
+      </c>
+      <c r="K9" s="22">
+        <v>5</v>
+      </c>
+      <c r="L9" s="22">
         <v>5</v>
       </c>
       <c r="M9" s="6">
@@ -1124,31 +1130,31 @@
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5">
-        <v>5</v>
-      </c>
-      <c r="F10" s="5">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5">
-        <v>5</v>
-      </c>
-      <c r="I10" s="5">
-        <v>5</v>
-      </c>
-      <c r="J10" s="5">
-        <v>5</v>
-      </c>
-      <c r="K10" s="5">
-        <v>5</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="D10" s="23">
+        <v>5</v>
+      </c>
+      <c r="E10" s="23">
+        <v>5</v>
+      </c>
+      <c r="F10" s="23">
+        <v>5</v>
+      </c>
+      <c r="G10" s="23">
+        <v>5</v>
+      </c>
+      <c r="H10" s="23">
+        <v>5</v>
+      </c>
+      <c r="I10" s="23">
+        <v>5</v>
+      </c>
+      <c r="J10" s="23">
+        <v>5</v>
+      </c>
+      <c r="K10" s="23">
+        <v>5</v>
+      </c>
+      <c r="L10" s="23">
         <v>5</v>
       </c>
       <c r="M10" s="6">
@@ -1190,31 +1196,31 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="20">
-        <v>5</v>
-      </c>
-      <c r="E11" s="20">
-        <v>5</v>
-      </c>
-      <c r="F11" s="20">
-        <v>5</v>
-      </c>
-      <c r="G11" s="20">
-        <v>5</v>
-      </c>
-      <c r="H11" s="20">
-        <v>5</v>
-      </c>
-      <c r="I11" s="20">
-        <v>5</v>
-      </c>
-      <c r="J11" s="23">
-        <v>5</v>
-      </c>
-      <c r="K11" s="23">
-        <v>5</v>
-      </c>
-      <c r="L11" s="23">
+      <c r="D11" s="19">
+        <v>5</v>
+      </c>
+      <c r="E11" s="19">
+        <v>5</v>
+      </c>
+      <c r="F11" s="19">
+        <v>5</v>
+      </c>
+      <c r="G11" s="19">
+        <v>5</v>
+      </c>
+      <c r="H11" s="19">
+        <v>5</v>
+      </c>
+      <c r="I11" s="19">
+        <v>5</v>
+      </c>
+      <c r="J11" s="22">
+        <v>5</v>
+      </c>
+      <c r="K11" s="22">
+        <v>5</v>
+      </c>
+      <c r="L11" s="22">
         <v>5</v>
       </c>
       <c r="M11" s="6">
@@ -1256,31 +1262,31 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="20">
-        <v>5</v>
-      </c>
-      <c r="E12" s="20">
-        <v>5</v>
-      </c>
-      <c r="F12" s="20">
-        <v>5</v>
-      </c>
-      <c r="G12" s="20">
-        <v>5</v>
-      </c>
-      <c r="H12" s="20">
-        <v>5</v>
-      </c>
-      <c r="I12" s="20">
-        <v>5</v>
-      </c>
-      <c r="J12" s="23">
-        <v>5</v>
-      </c>
-      <c r="K12" s="23">
-        <v>5</v>
-      </c>
-      <c r="L12" s="23">
+      <c r="D12" s="19">
+        <v>5</v>
+      </c>
+      <c r="E12" s="19">
+        <v>5</v>
+      </c>
+      <c r="F12" s="19">
+        <v>5</v>
+      </c>
+      <c r="G12" s="19">
+        <v>5</v>
+      </c>
+      <c r="H12" s="19">
+        <v>5</v>
+      </c>
+      <c r="I12" s="19">
+        <v>5</v>
+      </c>
+      <c r="J12" s="22">
+        <v>5</v>
+      </c>
+      <c r="K12" s="22">
+        <v>5</v>
+      </c>
+      <c r="L12" s="22">
         <v>5</v>
       </c>
       <c r="M12" s="6">
@@ -1322,31 +1328,31 @@
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="20">
-        <v>5</v>
-      </c>
-      <c r="E13" s="20">
-        <v>5</v>
-      </c>
-      <c r="F13" s="20">
-        <v>5</v>
-      </c>
-      <c r="G13" s="20">
-        <v>5</v>
-      </c>
-      <c r="H13" s="20">
-        <v>5</v>
-      </c>
-      <c r="I13" s="20">
-        <v>5</v>
-      </c>
-      <c r="J13" s="23">
-        <v>5</v>
-      </c>
-      <c r="K13" s="23">
-        <v>5</v>
-      </c>
-      <c r="L13" s="23">
+      <c r="D13" s="19">
+        <v>5</v>
+      </c>
+      <c r="E13" s="19">
+        <v>5</v>
+      </c>
+      <c r="F13" s="19">
+        <v>5</v>
+      </c>
+      <c r="G13" s="19">
+        <v>5</v>
+      </c>
+      <c r="H13" s="19">
+        <v>5</v>
+      </c>
+      <c r="I13" s="19">
+        <v>5</v>
+      </c>
+      <c r="J13" s="22">
+        <v>5</v>
+      </c>
+      <c r="K13" s="22">
+        <v>5</v>
+      </c>
+      <c r="L13" s="22">
         <v>5</v>
       </c>
       <c r="M13" s="6">
@@ -1388,31 +1394,31 @@
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="20">
-        <v>5</v>
-      </c>
-      <c r="E14" s="20">
-        <v>5</v>
-      </c>
-      <c r="F14" s="20">
-        <v>5</v>
-      </c>
-      <c r="G14" s="20">
-        <v>5</v>
-      </c>
-      <c r="H14" s="20">
-        <v>5</v>
-      </c>
-      <c r="I14" s="20">
-        <v>5</v>
-      </c>
-      <c r="J14" s="23">
-        <v>5</v>
-      </c>
-      <c r="K14" s="23">
-        <v>5</v>
-      </c>
-      <c r="L14" s="23">
+      <c r="D14" s="19">
+        <v>5</v>
+      </c>
+      <c r="E14" s="19">
+        <v>5</v>
+      </c>
+      <c r="F14" s="19">
+        <v>5</v>
+      </c>
+      <c r="G14" s="19">
+        <v>5</v>
+      </c>
+      <c r="H14" s="19">
+        <v>5</v>
+      </c>
+      <c r="I14" s="19">
+        <v>5</v>
+      </c>
+      <c r="J14" s="22">
+        <v>5</v>
+      </c>
+      <c r="K14" s="22">
+        <v>5</v>
+      </c>
+      <c r="L14" s="22">
         <v>5</v>
       </c>
       <c r="M14" s="6">
@@ -1454,28 +1460,28 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5">
-        <v>5</v>
-      </c>
-      <c r="E15" s="5">
-        <v>5</v>
-      </c>
-      <c r="F15" s="5">
-        <v>5</v>
-      </c>
-      <c r="G15" s="6">
-        <v>5</v>
-      </c>
-      <c r="H15" s="6">
-        <v>5</v>
-      </c>
-      <c r="I15" s="6">
-        <v>5</v>
-      </c>
-      <c r="J15" s="6">
-        <v>5</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="D15" s="23">
+        <v>5</v>
+      </c>
+      <c r="E15" s="23">
+        <v>5</v>
+      </c>
+      <c r="F15" s="23">
+        <v>5</v>
+      </c>
+      <c r="G15" s="24">
+        <v>5</v>
+      </c>
+      <c r="H15" s="24">
+        <v>5</v>
+      </c>
+      <c r="I15" s="24">
+        <v>5</v>
+      </c>
+      <c r="J15" s="24">
+        <v>5</v>
+      </c>
+      <c r="K15" s="24">
         <v>5</v>
       </c>
       <c r="L15" s="6"/>
@@ -1518,31 +1524,31 @@
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="20">
-        <v>5</v>
-      </c>
-      <c r="E16" s="20">
-        <v>5</v>
-      </c>
-      <c r="F16" s="20">
-        <v>5</v>
-      </c>
-      <c r="G16" s="20">
-        <v>5</v>
-      </c>
-      <c r="H16" s="20">
-        <v>5</v>
-      </c>
-      <c r="I16" s="20">
-        <v>5</v>
-      </c>
-      <c r="J16" s="23">
-        <v>5</v>
-      </c>
-      <c r="K16" s="23">
-        <v>5</v>
-      </c>
-      <c r="L16" s="23">
+      <c r="D16" s="19">
+        <v>5</v>
+      </c>
+      <c r="E16" s="19">
+        <v>5</v>
+      </c>
+      <c r="F16" s="19">
+        <v>5</v>
+      </c>
+      <c r="G16" s="19">
+        <v>5</v>
+      </c>
+      <c r="H16" s="19">
+        <v>5</v>
+      </c>
+      <c r="I16" s="19">
+        <v>5</v>
+      </c>
+      <c r="J16" s="22">
+        <v>5</v>
+      </c>
+      <c r="K16" s="22">
+        <v>5</v>
+      </c>
+      <c r="L16" s="22">
         <v>5</v>
       </c>
       <c r="M16" s="6">
@@ -1584,31 +1590,31 @@
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="20">
-        <v>5</v>
-      </c>
-      <c r="E17" s="17">
-        <v>5</v>
-      </c>
-      <c r="F17" s="17">
-        <v>5</v>
-      </c>
-      <c r="G17" s="17">
-        <v>5</v>
-      </c>
-      <c r="H17" s="17">
-        <v>5</v>
-      </c>
-      <c r="I17" s="17">
-        <v>5</v>
-      </c>
-      <c r="J17" s="17">
-        <v>5</v>
-      </c>
-      <c r="K17" s="17">
-        <v>5</v>
-      </c>
-      <c r="L17" s="17">
+      <c r="D17" s="19">
+        <v>5</v>
+      </c>
+      <c r="E17" s="25">
+        <v>5</v>
+      </c>
+      <c r="F17" s="25">
+        <v>5</v>
+      </c>
+      <c r="G17" s="25">
+        <v>5</v>
+      </c>
+      <c r="H17" s="25">
+        <v>5</v>
+      </c>
+      <c r="I17" s="25">
+        <v>5</v>
+      </c>
+      <c r="J17" s="25">
+        <v>5</v>
+      </c>
+      <c r="K17" s="25">
+        <v>5</v>
+      </c>
+      <c r="L17" s="25">
         <v>5</v>
       </c>
       <c r="M17" s="6">
@@ -1650,31 +1656,31 @@
       <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="20">
-        <v>5</v>
-      </c>
-      <c r="E18" s="20">
-        <v>5</v>
-      </c>
-      <c r="F18" s="20">
-        <v>5</v>
-      </c>
-      <c r="G18" s="20">
-        <v>5</v>
-      </c>
-      <c r="H18" s="20">
-        <v>5</v>
-      </c>
-      <c r="I18" s="20">
-        <v>5</v>
-      </c>
-      <c r="J18" s="22" t="s">
+      <c r="D18" s="19">
+        <v>5</v>
+      </c>
+      <c r="E18" s="19">
+        <v>5</v>
+      </c>
+      <c r="F18" s="19">
+        <v>5</v>
+      </c>
+      <c r="G18" s="19">
+        <v>5</v>
+      </c>
+      <c r="H18" s="19">
+        <v>5</v>
+      </c>
+      <c r="I18" s="19">
+        <v>5</v>
+      </c>
+      <c r="J18" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="17">
-        <v>5</v>
-      </c>
-      <c r="L18" s="17">
+      <c r="K18" s="25">
+        <v>5</v>
+      </c>
+      <c r="L18" s="25">
         <v>5</v>
       </c>
       <c r="M18" s="6">
@@ -1716,31 +1722,31 @@
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="20">
-        <v>5</v>
-      </c>
-      <c r="E19" s="20">
-        <v>5</v>
-      </c>
-      <c r="F19" s="20">
-        <v>5</v>
-      </c>
-      <c r="G19" s="21">
-        <v>5</v>
-      </c>
-      <c r="H19" s="20">
-        <v>5</v>
-      </c>
-      <c r="I19" s="20">
-        <v>5</v>
-      </c>
-      <c r="J19" s="23">
-        <v>5</v>
-      </c>
-      <c r="K19" s="22">
-        <v>5</v>
-      </c>
-      <c r="L19" s="22">
+      <c r="D19" s="19">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19">
+        <v>5</v>
+      </c>
+      <c r="F19" s="19">
+        <v>5</v>
+      </c>
+      <c r="G19" s="20">
+        <v>5</v>
+      </c>
+      <c r="H19" s="19">
+        <v>5</v>
+      </c>
+      <c r="I19" s="19">
+        <v>5</v>
+      </c>
+      <c r="J19" s="22">
+        <v>5</v>
+      </c>
+      <c r="K19" s="21">
+        <v>5</v>
+      </c>
+      <c r="L19" s="21">
         <v>5</v>
       </c>
       <c r="M19" s="6">
@@ -1782,31 +1788,31 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="24">
-        <v>5</v>
-      </c>
-      <c r="E20" s="25">
-        <v>5</v>
-      </c>
-      <c r="F20" s="25">
-        <v>5</v>
-      </c>
-      <c r="G20" s="25">
-        <v>5</v>
-      </c>
-      <c r="H20" s="25">
-        <v>5</v>
-      </c>
-      <c r="I20" s="25">
-        <v>5</v>
-      </c>
-      <c r="J20" s="25">
-        <v>5</v>
-      </c>
-      <c r="K20" s="25">
-        <v>5</v>
-      </c>
-      <c r="L20" s="25">
+      <c r="D20" s="26">
+        <v>5</v>
+      </c>
+      <c r="E20" s="27">
+        <v>5</v>
+      </c>
+      <c r="F20" s="27">
+        <v>5</v>
+      </c>
+      <c r="G20" s="27">
+        <v>5</v>
+      </c>
+      <c r="H20" s="27">
+        <v>5</v>
+      </c>
+      <c r="I20" s="27">
+        <v>5</v>
+      </c>
+      <c r="J20" s="27">
+        <v>5</v>
+      </c>
+      <c r="K20" s="27">
+        <v>5</v>
+      </c>
+      <c r="L20" s="27">
         <v>5</v>
       </c>
       <c r="M20" s="6">
@@ -1848,29 +1854,29 @@
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
         <v>5</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="20">
-        <v>5</v>
-      </c>
-      <c r="G21" s="20">
-        <v>5</v>
-      </c>
-      <c r="H21" s="20">
-        <v>5</v>
-      </c>
-      <c r="I21" s="20">
-        <v>5</v>
-      </c>
-      <c r="J21" s="23">
-        <v>5</v>
-      </c>
-      <c r="K21" s="3">
-        <v>5</v>
-      </c>
-      <c r="L21" s="3">
+      <c r="F21" s="19">
+        <v>5</v>
+      </c>
+      <c r="G21" s="19">
+        <v>5</v>
+      </c>
+      <c r="H21" s="19">
+        <v>5</v>
+      </c>
+      <c r="I21" s="19">
+        <v>5</v>
+      </c>
+      <c r="J21" s="22">
+        <v>5</v>
+      </c>
+      <c r="K21" s="28">
+        <v>5</v>
+      </c>
+      <c r="L21" s="28">
         <v>5</v>
       </c>
       <c r="M21" s="6">
@@ -1912,31 +1918,31 @@
       <c r="C22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="20">
-        <v>5</v>
-      </c>
-      <c r="E22" s="20">
-        <v>5</v>
-      </c>
-      <c r="F22" s="20">
-        <v>5</v>
-      </c>
-      <c r="G22" s="20">
-        <v>5</v>
-      </c>
-      <c r="H22" s="20">
-        <v>5</v>
-      </c>
-      <c r="I22" s="20">
-        <v>5</v>
-      </c>
-      <c r="J22" s="23">
-        <v>5</v>
-      </c>
-      <c r="K22" s="23">
-        <v>5</v>
-      </c>
-      <c r="L22" s="23">
+      <c r="D22" s="19">
+        <v>5</v>
+      </c>
+      <c r="E22" s="19">
+        <v>5</v>
+      </c>
+      <c r="F22" s="19">
+        <v>5</v>
+      </c>
+      <c r="G22" s="19">
+        <v>5</v>
+      </c>
+      <c r="H22" s="19">
+        <v>5</v>
+      </c>
+      <c r="I22" s="19">
+        <v>5</v>
+      </c>
+      <c r="J22" s="22">
+        <v>5</v>
+      </c>
+      <c r="K22" s="22">
+        <v>5</v>
+      </c>
+      <c r="L22" s="22">
         <v>5</v>
       </c>
       <c r="M22" s="6">
@@ -1978,31 +1984,31 @@
       <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="20">
-        <v>5</v>
-      </c>
-      <c r="E23" s="20">
-        <v>5</v>
-      </c>
-      <c r="F23" s="20">
-        <v>5</v>
-      </c>
-      <c r="G23" s="20">
-        <v>5</v>
-      </c>
-      <c r="H23" s="20">
-        <v>5</v>
-      </c>
-      <c r="I23" s="20">
-        <v>5</v>
-      </c>
-      <c r="J23" s="6">
-        <v>5</v>
-      </c>
-      <c r="K23" s="6">
-        <v>5</v>
-      </c>
-      <c r="L23" s="6">
+      <c r="D23" s="19">
+        <v>5</v>
+      </c>
+      <c r="E23" s="19">
+        <v>5</v>
+      </c>
+      <c r="F23" s="19">
+        <v>5</v>
+      </c>
+      <c r="G23" s="19">
+        <v>5</v>
+      </c>
+      <c r="H23" s="19">
+        <v>5</v>
+      </c>
+      <c r="I23" s="19">
+        <v>5</v>
+      </c>
+      <c r="J23" s="24">
+        <v>5</v>
+      </c>
+      <c r="K23" s="24">
+        <v>5</v>
+      </c>
+      <c r="L23" s="24">
         <v>5</v>
       </c>
       <c r="M23" s="6">
@@ -2044,31 +2050,31 @@
       <c r="C24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="20">
-        <v>5</v>
-      </c>
-      <c r="E24" s="20">
-        <v>5</v>
-      </c>
-      <c r="F24" s="20">
-        <v>5</v>
-      </c>
-      <c r="G24" s="20">
-        <v>5</v>
-      </c>
-      <c r="H24" s="20">
-        <v>5</v>
-      </c>
-      <c r="I24" s="20">
-        <v>5</v>
-      </c>
-      <c r="J24" s="23">
-        <v>5</v>
-      </c>
-      <c r="K24" s="23">
-        <v>5</v>
-      </c>
-      <c r="L24" s="23">
+      <c r="D24" s="19">
+        <v>5</v>
+      </c>
+      <c r="E24" s="19">
+        <v>5</v>
+      </c>
+      <c r="F24" s="19">
+        <v>5</v>
+      </c>
+      <c r="G24" s="19">
+        <v>5</v>
+      </c>
+      <c r="H24" s="19">
+        <v>5</v>
+      </c>
+      <c r="I24" s="19">
+        <v>5</v>
+      </c>
+      <c r="J24" s="22">
+        <v>5</v>
+      </c>
+      <c r="K24" s="22">
+        <v>5</v>
+      </c>
+      <c r="L24" s="22">
         <v>5</v>
       </c>
       <c r="M24" s="6">
@@ -2110,31 +2116,31 @@
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="20">
-        <v>5</v>
-      </c>
-      <c r="E25" s="20">
-        <v>5</v>
-      </c>
-      <c r="F25" s="20">
-        <v>5</v>
-      </c>
-      <c r="G25" s="20">
-        <v>5</v>
-      </c>
-      <c r="H25" s="20">
-        <v>5</v>
-      </c>
-      <c r="I25" s="20">
-        <v>5</v>
-      </c>
-      <c r="J25" s="23">
-        <v>5</v>
-      </c>
-      <c r="K25" s="23">
-        <v>5</v>
-      </c>
-      <c r="L25" s="23">
+      <c r="D25" s="19">
+        <v>5</v>
+      </c>
+      <c r="E25" s="19">
+        <v>5</v>
+      </c>
+      <c r="F25" s="19">
+        <v>5</v>
+      </c>
+      <c r="G25" s="19">
+        <v>5</v>
+      </c>
+      <c r="H25" s="19">
+        <v>5</v>
+      </c>
+      <c r="I25" s="19">
+        <v>5</v>
+      </c>
+      <c r="J25" s="22">
+        <v>5</v>
+      </c>
+      <c r="K25" s="22">
+        <v>5</v>
+      </c>
+      <c r="L25" s="22">
         <v>5</v>
       </c>
       <c r="M25" s="6">
@@ -2176,31 +2182,31 @@
       <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="20">
-        <v>5</v>
-      </c>
-      <c r="E26" s="20">
-        <v>5</v>
-      </c>
-      <c r="F26" s="20">
-        <v>5</v>
-      </c>
-      <c r="G26" s="20">
-        <v>5</v>
-      </c>
-      <c r="H26" s="20">
-        <v>5</v>
-      </c>
-      <c r="I26" s="20">
-        <v>5</v>
-      </c>
-      <c r="J26" s="23">
-        <v>5</v>
-      </c>
-      <c r="K26" s="23">
-        <v>5</v>
-      </c>
-      <c r="L26" s="23">
+      <c r="D26" s="19">
+        <v>5</v>
+      </c>
+      <c r="E26" s="19">
+        <v>5</v>
+      </c>
+      <c r="F26" s="19">
+        <v>5</v>
+      </c>
+      <c r="G26" s="19">
+        <v>5</v>
+      </c>
+      <c r="H26" s="19">
+        <v>5</v>
+      </c>
+      <c r="I26" s="19">
+        <v>5</v>
+      </c>
+      <c r="J26" s="22">
+        <v>5</v>
+      </c>
+      <c r="K26" s="22">
+        <v>5</v>
+      </c>
+      <c r="L26" s="22">
         <v>5</v>
       </c>
       <c r="M26" s="6">
@@ -2289,31 +2295,31 @@
       <c r="C28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="20">
-        <v>5</v>
-      </c>
-      <c r="E28" s="20">
-        <v>5</v>
-      </c>
-      <c r="F28" s="20">
-        <v>5</v>
-      </c>
-      <c r="G28" s="20">
-        <v>5</v>
-      </c>
-      <c r="H28" s="20">
-        <v>5</v>
-      </c>
-      <c r="I28" s="20">
-        <v>5</v>
-      </c>
-      <c r="J28" s="23">
-        <v>5</v>
-      </c>
-      <c r="K28" s="17">
-        <v>5</v>
-      </c>
-      <c r="L28" s="17">
+      <c r="D28" s="19">
+        <v>5</v>
+      </c>
+      <c r="E28" s="19">
+        <v>5</v>
+      </c>
+      <c r="F28" s="19">
+        <v>5</v>
+      </c>
+      <c r="G28" s="19">
+        <v>5</v>
+      </c>
+      <c r="H28" s="19">
+        <v>5</v>
+      </c>
+      <c r="I28" s="19">
+        <v>5</v>
+      </c>
+      <c r="J28" s="22">
+        <v>5</v>
+      </c>
+      <c r="K28" s="25">
+        <v>5</v>
+      </c>
+      <c r="L28" s="25">
         <v>5</v>
       </c>
       <c r="M28" s="6">
@@ -2355,31 +2361,31 @@
       <c r="C29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="20">
-        <v>5</v>
-      </c>
-      <c r="E29" s="20">
-        <v>5</v>
-      </c>
-      <c r="F29" s="20">
-        <v>5</v>
-      </c>
-      <c r="G29" s="20">
-        <v>5</v>
-      </c>
-      <c r="H29" s="20">
-        <v>5</v>
-      </c>
-      <c r="I29" s="20">
-        <v>5</v>
-      </c>
-      <c r="J29" s="23">
-        <v>5</v>
-      </c>
-      <c r="K29" s="23">
-        <v>5</v>
-      </c>
-      <c r="L29" s="23">
+      <c r="D29" s="19">
+        <v>5</v>
+      </c>
+      <c r="E29" s="19">
+        <v>5</v>
+      </c>
+      <c r="F29" s="19">
+        <v>5</v>
+      </c>
+      <c r="G29" s="19">
+        <v>5</v>
+      </c>
+      <c r="H29" s="19">
+        <v>5</v>
+      </c>
+      <c r="I29" s="19">
+        <v>5</v>
+      </c>
+      <c r="J29" s="22">
+        <v>5</v>
+      </c>
+      <c r="K29" s="22">
+        <v>5</v>
+      </c>
+      <c r="L29" s="22">
         <v>5</v>
       </c>
       <c r="M29" s="6">
@@ -2421,31 +2427,31 @@
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="20">
-        <v>5</v>
-      </c>
-      <c r="E30" s="20">
-        <v>5</v>
-      </c>
-      <c r="F30" s="20">
-        <v>5</v>
-      </c>
-      <c r="G30" s="21">
-        <v>5</v>
-      </c>
-      <c r="H30" s="20">
-        <v>5</v>
-      </c>
-      <c r="I30" s="20">
-        <v>5</v>
-      </c>
-      <c r="J30" s="23">
-        <v>5</v>
-      </c>
-      <c r="K30" s="23">
-        <v>5</v>
-      </c>
-      <c r="L30" s="23">
+      <c r="D30" s="19">
+        <v>5</v>
+      </c>
+      <c r="E30" s="19">
+        <v>5</v>
+      </c>
+      <c r="F30" s="19">
+        <v>5</v>
+      </c>
+      <c r="G30" s="20">
+        <v>5</v>
+      </c>
+      <c r="H30" s="19">
+        <v>5</v>
+      </c>
+      <c r="I30" s="19">
+        <v>5</v>
+      </c>
+      <c r="J30" s="22">
+        <v>5</v>
+      </c>
+      <c r="K30" s="22">
+        <v>5</v>
+      </c>
+      <c r="L30" s="22">
         <v>5</v>
       </c>
       <c r="M30" s="6">
@@ -2487,22 +2493,22 @@
       <c r="C31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="20">
-        <v>5</v>
-      </c>
-      <c r="E31" s="20">
-        <v>5</v>
-      </c>
-      <c r="F31" s="20">
-        <v>5</v>
-      </c>
-      <c r="G31" s="20">
-        <v>5</v>
-      </c>
-      <c r="H31" s="20">
-        <v>5</v>
-      </c>
-      <c r="I31" s="20">
+      <c r="D31" s="19">
+        <v>5</v>
+      </c>
+      <c r="E31" s="19">
+        <v>5</v>
+      </c>
+      <c r="F31" s="19">
+        <v>5</v>
+      </c>
+      <c r="G31" s="19">
+        <v>5</v>
+      </c>
+      <c r="H31" s="19">
+        <v>5</v>
+      </c>
+      <c r="I31" s="19">
         <v>5</v>
       </c>
       <c r="J31" s="7"/>
@@ -2549,31 +2555,31 @@
       <c r="C32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="20">
-        <v>5</v>
-      </c>
-      <c r="E32" s="5">
-        <v>5</v>
-      </c>
-      <c r="F32" s="20">
-        <v>5</v>
-      </c>
-      <c r="G32" s="17">
-        <v>5</v>
-      </c>
-      <c r="H32" s="20">
-        <v>5</v>
-      </c>
-      <c r="I32" s="20">
-        <v>5</v>
-      </c>
-      <c r="J32" s="17">
-        <v>5</v>
-      </c>
-      <c r="K32" s="17">
-        <v>5</v>
-      </c>
-      <c r="L32" s="17">
+      <c r="D32" s="19">
+        <v>5</v>
+      </c>
+      <c r="E32" s="23">
+        <v>5</v>
+      </c>
+      <c r="F32" s="23">
+        <v>5</v>
+      </c>
+      <c r="G32" s="25">
+        <v>5</v>
+      </c>
+      <c r="H32" s="23">
+        <v>5</v>
+      </c>
+      <c r="I32" s="23">
+        <v>5</v>
+      </c>
+      <c r="J32" s="25">
+        <v>5</v>
+      </c>
+      <c r="K32" s="25">
+        <v>5</v>
+      </c>
+      <c r="L32" s="25">
         <v>5</v>
       </c>
       <c r="M32" s="6">
@@ -2615,31 +2621,31 @@
       <c r="C33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="20">
-        <v>5</v>
-      </c>
-      <c r="E33" s="20">
-        <v>5</v>
-      </c>
-      <c r="F33" s="3">
-        <v>5</v>
-      </c>
-      <c r="G33" s="20">
-        <v>5</v>
-      </c>
-      <c r="H33" s="3">
-        <v>5</v>
-      </c>
-      <c r="I33" s="3">
-        <v>5</v>
-      </c>
-      <c r="J33" s="3">
-        <v>5</v>
-      </c>
-      <c r="K33" s="3">
-        <v>5</v>
-      </c>
-      <c r="L33" s="3">
+      <c r="D33" s="19">
+        <v>5</v>
+      </c>
+      <c r="E33" s="19">
+        <v>5</v>
+      </c>
+      <c r="F33" s="28">
+        <v>5</v>
+      </c>
+      <c r="G33" s="23">
+        <v>5</v>
+      </c>
+      <c r="H33" s="28">
+        <v>5</v>
+      </c>
+      <c r="I33" s="28">
+        <v>5</v>
+      </c>
+      <c r="J33" s="28">
+        <v>5</v>
+      </c>
+      <c r="K33" s="28">
+        <v>5</v>
+      </c>
+      <c r="L33" s="28">
         <v>5</v>
       </c>
       <c r="M33" s="6">
@@ -2670,148 +2676,703 @@
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23" ht="18.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D34" s="18">
-        <v>1</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="18.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="19">
+        <v>5</v>
+      </c>
+      <c r="E34" s="19">
+        <v>5</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+      <c r="G34" s="19">
+        <v>5</v>
+      </c>
+      <c r="H34" s="3">
+        <v>5</v>
+      </c>
+      <c r="I34" s="3">
+        <v>5</v>
+      </c>
+      <c r="J34" s="3">
+        <v>5</v>
+      </c>
+      <c r="K34" s="3">
+        <v>5</v>
+      </c>
+      <c r="L34" s="3">
+        <v>5</v>
+      </c>
+      <c r="M34" s="6">
+        <v>2</v>
+      </c>
+      <c r="N34" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P34" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R34" s="4"/>
+      <c r="S34" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="19">
+        <v>5</v>
+      </c>
+      <c r="E35" s="19">
+        <v>5</v>
+      </c>
+      <c r="F35" s="3">
+        <v>5</v>
+      </c>
+      <c r="G35" s="19">
+        <v>5</v>
+      </c>
+      <c r="H35" s="3">
+        <v>5</v>
+      </c>
+      <c r="I35" s="3">
+        <v>5</v>
+      </c>
+      <c r="J35" s="3">
+        <v>5</v>
+      </c>
+      <c r="K35" s="3">
+        <v>5</v>
+      </c>
+      <c r="L35" s="3">
+        <v>5</v>
+      </c>
+      <c r="M35" s="6">
+        <v>2</v>
+      </c>
+      <c r="N35" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P35" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R35" s="4"/>
+      <c r="S35" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="19">
+        <v>5</v>
+      </c>
+      <c r="E36" s="19">
+        <v>5</v>
+      </c>
+      <c r="F36" s="3">
+        <v>5</v>
+      </c>
+      <c r="G36" s="19">
+        <v>5</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5</v>
+      </c>
+      <c r="I36" s="3">
+        <v>5</v>
+      </c>
+      <c r="J36" s="3">
+        <v>5</v>
+      </c>
+      <c r="K36" s="3">
+        <v>5</v>
+      </c>
+      <c r="L36" s="3">
+        <v>5</v>
+      </c>
+      <c r="M36" s="6">
+        <v>2</v>
+      </c>
+      <c r="N36" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P36" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="4"/>
+      <c r="S36" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="19">
+        <v>5</v>
+      </c>
+      <c r="E37" s="19">
+        <v>5</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="19">
+        <v>5</v>
+      </c>
+      <c r="H37" s="3">
+        <v>5</v>
+      </c>
+      <c r="I37" s="3">
+        <v>5</v>
+      </c>
+      <c r="J37" s="3">
+        <v>5</v>
+      </c>
+      <c r="K37" s="3">
+        <v>5</v>
+      </c>
+      <c r="L37" s="3">
+        <v>5</v>
+      </c>
+      <c r="M37" s="6">
+        <v>2</v>
+      </c>
+      <c r="N37" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P37" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R37" s="4"/>
+      <c r="S37" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="19">
+        <v>5</v>
+      </c>
+      <c r="E38" s="19">
+        <v>5</v>
+      </c>
+      <c r="F38" s="3">
+        <v>5</v>
+      </c>
+      <c r="G38" s="19">
+        <v>5</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5</v>
+      </c>
+      <c r="I38" s="3">
+        <v>5</v>
+      </c>
+      <c r="J38" s="3">
+        <v>5</v>
+      </c>
+      <c r="K38" s="3">
+        <v>5</v>
+      </c>
+      <c r="L38" s="3">
+        <v>5</v>
+      </c>
+      <c r="M38" s="6">
+        <v>2</v>
+      </c>
+      <c r="N38" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P38" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="4"/>
+      <c r="S38" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="19">
+        <v>5</v>
+      </c>
+      <c r="E39" s="19">
+        <v>5</v>
+      </c>
+      <c r="F39" s="3">
+        <v>5</v>
+      </c>
+      <c r="G39" s="19">
+        <v>5</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5</v>
+      </c>
+      <c r="I39" s="3">
+        <v>5</v>
+      </c>
+      <c r="J39" s="3">
+        <v>5</v>
+      </c>
+      <c r="K39" s="3">
+        <v>5</v>
+      </c>
+      <c r="L39" s="3">
+        <v>5</v>
+      </c>
+      <c r="M39" s="6">
+        <v>2</v>
+      </c>
+      <c r="N39" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P39" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="4"/>
+      <c r="S39" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="19">
+        <v>5</v>
+      </c>
+      <c r="E40" s="19">
+        <v>5</v>
+      </c>
+      <c r="F40" s="3">
+        <v>5</v>
+      </c>
+      <c r="G40" s="19">
+        <v>5</v>
+      </c>
+      <c r="H40" s="3">
+        <v>5</v>
+      </c>
+      <c r="I40" s="3">
+        <v>5</v>
+      </c>
+      <c r="J40" s="3">
+        <v>5</v>
+      </c>
+      <c r="K40" s="3">
+        <v>5</v>
+      </c>
+      <c r="L40" s="3">
+        <v>5</v>
+      </c>
+      <c r="M40" s="6">
+        <v>2</v>
+      </c>
+      <c r="N40" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P40" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="4"/>
+      <c r="S40" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="19">
+        <v>5</v>
+      </c>
+      <c r="E41" s="19">
+        <v>5</v>
+      </c>
+      <c r="F41" s="3">
+        <v>5</v>
+      </c>
+      <c r="G41" s="19">
+        <v>5</v>
+      </c>
+      <c r="H41" s="3">
+        <v>5</v>
+      </c>
+      <c r="I41" s="3">
+        <v>5</v>
+      </c>
+      <c r="J41" s="3">
+        <v>5</v>
+      </c>
+      <c r="K41" s="3">
+        <v>5</v>
+      </c>
+      <c r="L41" s="3">
+        <v>5</v>
+      </c>
+      <c r="M41" s="6">
+        <v>2</v>
+      </c>
+      <c r="N41" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O41" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P41" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R41" s="4"/>
+      <c r="S41" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="19">
+        <v>5</v>
+      </c>
+      <c r="E42" s="19">
+        <v>5</v>
+      </c>
+      <c r="F42" s="3">
+        <v>5</v>
+      </c>
+      <c r="G42" s="19">
+        <v>5</v>
+      </c>
+      <c r="H42" s="3">
+        <v>5</v>
+      </c>
+      <c r="I42" s="3">
+        <v>5</v>
+      </c>
+      <c r="J42" s="3">
+        <v>5</v>
+      </c>
+      <c r="K42" s="3">
+        <v>5</v>
+      </c>
+      <c r="L42" s="3">
+        <v>5</v>
+      </c>
+      <c r="M42" s="6">
+        <v>2</v>
+      </c>
+      <c r="N42" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O42" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P42" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R42" s="4"/>
+      <c r="S42" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="19">
+        <v>5</v>
+      </c>
+      <c r="E43" s="19">
+        <v>5</v>
+      </c>
+      <c r="F43" s="3">
+        <v>5</v>
+      </c>
+      <c r="G43" s="19">
+        <v>5</v>
+      </c>
+      <c r="H43" s="3">
+        <v>5</v>
+      </c>
+      <c r="I43" s="3">
+        <v>5</v>
+      </c>
+      <c r="J43" s="3">
+        <v>5</v>
+      </c>
+      <c r="K43" s="3">
+        <v>5</v>
+      </c>
+      <c r="L43" s="3">
+        <v>5</v>
+      </c>
+      <c r="M43" s="6">
+        <v>2</v>
+      </c>
+      <c r="N43" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O43" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P43" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R43" s="4"/>
+      <c r="S43" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="19">
+        <v>5</v>
+      </c>
+      <c r="E44" s="19">
+        <v>5</v>
+      </c>
+      <c r="F44" s="3">
+        <v>5</v>
+      </c>
+      <c r="G44" s="19">
+        <v>5</v>
+      </c>
+      <c r="H44" s="3">
+        <v>5</v>
+      </c>
+      <c r="I44" s="3">
+        <v>5</v>
+      </c>
+      <c r="J44" s="3">
+        <v>5</v>
+      </c>
+      <c r="K44" s="3">
+        <v>5</v>
+      </c>
+      <c r="L44" s="3">
+        <v>5</v>
+      </c>
+      <c r="M44" s="6">
+        <v>2</v>
+      </c>
+      <c r="N44" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P44" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="4"/>
+      <c r="S44" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="19">
+        <v>5</v>
+      </c>
+      <c r="E45" s="19">
+        <v>5</v>
+      </c>
+      <c r="F45" s="3">
+        <v>5</v>
+      </c>
+      <c r="G45" s="19">
+        <v>5</v>
+      </c>
+      <c r="H45" s="3">
+        <v>5</v>
+      </c>
+      <c r="I45" s="3">
+        <v>5</v>
+      </c>
+      <c r="J45" s="3">
+        <v>5</v>
+      </c>
+      <c r="K45" s="3">
+        <v>5</v>
+      </c>
+      <c r="L45" s="3">
+        <v>5</v>
+      </c>
+      <c r="M45" s="6">
+        <v>2</v>
+      </c>
+      <c r="N45" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O45" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P45" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R45" s="4"/>
+      <c r="S45" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>

</xml_diff>